<commit_message>
Update JSON for images 124-167
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1361,9 +1361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1401,7 +1401,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1507,7 +1507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1649,7 +1649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1659,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4443A7F1-90C3-4D7D-8B82-1D6A6D8DE156}">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C151" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135:G168"/>
+    <sheetView tabSelected="1" topLeftCell="C159" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125:G168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update lists to github.io
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/website/DALeske.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="8_{6B798D66-B0F0-4AC0-877C-232D0BFEA49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0021A96-8DEF-4050-9FE5-5902705CF730}"/>
+  <xr:revisionPtr revIDLastSave="577" documentId="8_{6B798D66-B0F0-4AC0-877C-232D0BFEA49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EB6CD85-8840-467F-BFC3-9AFC5A36E0CD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
   </bookViews>
@@ -793,507 +793,6 @@
     <t>Farmer's Market Trucks</t>
   </si>
   <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_123.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_002.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_003.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_004.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_005.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_007.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_008.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_009.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_011.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_013.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_014.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_015.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_016.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_017.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_018.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_019.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_020.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_021.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_022.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_023.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_024.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_025.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_026.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_027.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_028.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_029.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_030.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_031.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_032.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_033.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_035.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_036.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_038.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_039.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_040.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_041.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_042.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_043.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_044.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_045.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_046.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_047.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_048.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_050.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_051.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_052.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_053.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_054.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_055.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_056.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_057.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_058.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_059.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_060.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_061.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_062.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_063.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_064.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_065.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_066.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_067.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_069.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_071.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_073.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_075.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_076.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_077.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_078.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_079.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_080.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_081.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_082.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_083.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_084.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_085.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_086.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_087.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_088.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_089.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_090.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_092.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_093.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_094.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_095.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_096.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_097.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_098.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_099.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_100.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_101.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_102.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_103.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_104.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_105.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_106.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_107.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_108.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_109.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_110.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_111.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_112.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_113.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_114.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_115.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_116.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_117.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_118.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_119.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_120.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_121.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_122.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_124.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_125.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_126.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_127.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_128.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_129.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_130.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_131.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_132.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_133.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_134.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_135.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_136.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_137.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_138.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_139.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_140.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_141.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_142.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_143.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_144.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_145.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_146.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_147.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_148.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_149.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_150.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_151.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_152.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_153.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_154.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_155.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_156.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_157.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_158.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_159.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_160.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_161.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_162.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_163.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_164.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_165.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_166.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_167.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_001.JPG</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_006.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_010.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_012.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_034.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_037.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_049.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_068.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_070.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_072.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_074.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_091.jpeg</t>
-  </si>
-  <si>
     <t>JSON</t>
   </si>
   <si>
@@ -1342,28 +841,529 @@
     <t>35 X 27</t>
   </si>
   <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_172.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_173.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_174.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg</t>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_001.JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_002.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_003.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_004.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_005.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_006.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_007.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_008.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_009.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_010.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_011.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_012.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_013.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_014.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_015.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_016.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_017.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_018.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_019.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_020.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_021.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_022.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_023.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_024.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_025.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_026.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_027.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_028.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_029.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_030.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_031.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_032.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_033.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_034.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_035.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_036.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_037.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_038.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_039.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_040.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_041.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_042.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_043.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_044.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_045.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_046.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_047.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_048.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_049.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_050.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_051.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_052.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_053.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_054.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_055.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_056.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_057.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_058.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_059.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_060.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_061.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_062.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_063.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_064.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_065.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_066.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_067.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_068.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_069.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_070.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_071.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_072.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_073.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_074.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_075.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_076.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_077.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_078.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_079.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_080.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_081.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_082.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_083.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_084.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_085.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_086.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_087.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_088.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_089.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_090.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_091.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_092.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_093.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_094.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_095.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_096.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_097.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_098.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_099.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_100.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_101.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_102.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_103.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_104.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_105.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_106.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_107.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_108.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_109.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_110.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_111.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_112.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_113.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_114.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_115.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_116.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_117.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_118.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_119.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_120.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_121.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_122.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_123.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_124.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_125.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_126.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_127.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_128.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_129.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_130.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_131.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_132.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_133.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_134.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_135.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_136.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_137.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_138.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_139.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_140.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_141.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_142.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_143.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_144.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_145.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_146.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_147.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_148.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_149.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_150.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_151.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_152.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_153.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_154.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_155.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_156.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_157.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_158.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_159.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_160.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_161.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_162.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_163.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_164.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_165.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_166.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_167.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_168.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_169.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_170.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_171.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_172.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_173.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_174.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_175.jpg</t>
   </si>
 </sst>
 </file>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4443A7F1-90C3-4D7D-8B82-1D6A6D8DE156}">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C156" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169:G176"/>
+    <sheetView tabSelected="1" topLeftCell="C169" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,7 +1761,7 @@
         <v>191</v>
       </c>
       <c r="G1" t="s">
-        <v>418</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1781,11 +1781,11 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>406</v>
+        <v>267</v>
       </c>
       <c r="G2" t="str">
-        <f>CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F2&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "1","Title": "Lighthouse","Pieces": "500","Company": "Re-marks","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_001.JPG"</v>
+        <f>"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F2&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "1","Title": "Lighthouse","Pieces": "500","Company": "Re-marks","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_001.JPG"},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1805,11 +1805,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" si="0">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F3&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "2","Title": "Cakes","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_002.jpg"</v>
+        <f t="shared" ref="G3:G66" si="0">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F3&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "2","Title": "Cakes","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_002.jpg"},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1829,11 +1829,11 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "3","Title": "More Ice Cream Please","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_003.jpg"</v>
+        <v>{"PuzzleNum": "3","Title": "More Ice Cream Please","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_003.jpg"},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1853,11 +1853,11 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "4","Title": "Artsy Cats","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_004.jpg"</v>
+        <v>{"PuzzleNum": "4","Title": "Artsy Cats","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_004.jpg"},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1877,11 +1877,11 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "5","Title": "Air Mail","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_005.jpg"</v>
+        <v>{"PuzzleNum": "5","Title": "Air Mail","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_005.jpg"},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1901,11 +1901,11 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>407</v>
+        <v>272</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_006.jpeg"</v>
+        <v>{"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_006.jpeg"},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1925,11 +1925,11 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "7","Title": "Kitchen Cupboard","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_007.jpg"</v>
+        <v>{"PuzzleNum": "7","Title": "Kitchen Cupboard","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_007.jpg"},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1949,11 +1949,11 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "8","Title": "99 Beautiful Places","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_008.jpg"</v>
+        <v>{"PuzzleNum": "8","Title": "99 Beautiful Places","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_008.jpg"},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1973,11 +1973,11 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "9","Title": "Songbirds","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_009.jpg"</v>
+        <v>{"PuzzleNum": "9","Title": "Songbirds","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_009.jpg"},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1997,11 +1997,11 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>408</v>
+        <v>276</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "10","Title": "Marbles","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_010.jpeg"</v>
+        <v>{"PuzzleNum": "10","Title": "Marbles","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_010.jpeg"},</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2021,11 +2021,11 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "11","Title": "60 American National Parks","Pieces": "500","Company": "True South","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_011.jpg"</v>
+        <v>{"PuzzleNum": "11","Title": "60 American National Parks","Pieces": "500","Company": "True South","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_011.jpg"},</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2045,11 +2045,11 @@
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>409</v>
+        <v>278</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "12","Title": "Visting the Mansion","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_012.jpeg"</v>
+        <v>{"PuzzleNum": "12","Title": "Visting the Mansion","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_012.jpeg"},</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2069,11 +2069,11 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "13","Title": "Black Beauty Carousel Horse","Pieces": "500","Company": "Colorluxe","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_013.jpg"</v>
+        <v>{"PuzzleNum": "13","Title": "Black Beauty Carousel Horse","Pieces": "500","Company": "Colorluxe","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_013.jpg"},</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2093,11 +2093,11 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "14","Title": "Teddy Bear Workshop","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_014.jpg"</v>
+        <v>{"PuzzleNum": "14","Title": "Teddy Bear Workshop","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_014.jpg"},</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2117,11 +2117,11 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "15","Title": "Doughnuts","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_015.jpg"</v>
+        <v>{"PuzzleNum": "15","Title": "Doughnuts","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_015.jpg"},</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2141,11 +2141,11 @@
         <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "16","Title": "Pretty Birds","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_016.jpg"</v>
+        <v>{"PuzzleNum": "16","Title": "Pretty Birds","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_016.jpg"},</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2165,11 +2165,11 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "17","Title": "Bicycle","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_017.jpg"</v>
+        <v>{"PuzzleNum": "17","Title": "Bicycle","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_017.jpg"},</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2189,11 +2189,11 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "18","Title": "Spring Flowers","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_018.jpg"</v>
+        <v>{"PuzzleNum": "18","Title": "Spring Flowers","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_018.jpg"},</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2213,11 +2213,11 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "19","Title": "The Bizarre Workshop","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_019.jpg"</v>
+        <v>{"PuzzleNum": "19","Title": "The Bizarre Workshop","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_019.jpg"},</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2237,11 +2237,11 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "20","Title": "Floral Reflections","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_020.jpg"</v>
+        <v>{"PuzzleNum": "20","Title": "Floral Reflections","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_020.jpg"},</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2261,11 +2261,11 @@
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "21","Title": "Snack Treats","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_021.jpg"</v>
+        <v>{"PuzzleNum": "21","Title": "Snack Treats","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_021.jpg"},</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2285,11 +2285,11 @@
         <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "22","Title": "Oh Buoy!","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_022.jpg"</v>
+        <v>{"PuzzleNum": "22","Title": "Oh Buoy!","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_022.jpg"},</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2309,11 +2309,11 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "23","Title": "Colorful Yarn","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_023.jpg"</v>
+        <v>{"PuzzleNum": "23","Title": "Colorful Yarn","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_023.jpg"},</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2333,11 +2333,11 @@
         <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "24","Title": "Butterfly Frenzy","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_024.jpg"</v>
+        <v>{"PuzzleNum": "24","Title": "Butterfly Frenzy","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_024.jpg"},</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2357,11 +2357,11 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "25","Title": "Shelter From the Storm","Pieces": "500","Company": "Bits and Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_025.jpg"</v>
+        <v>{"PuzzleNum": "25","Title": "Shelter From the Storm","Pieces": "500","Company": "Bits and Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_025.jpg"},</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2381,11 +2381,11 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "26","Title": "Prima Ballerina","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_026.jpg"</v>
+        <v>{"PuzzleNum": "26","Title": "Prima Ballerina","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_026.jpg"},</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2405,11 +2405,11 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "27","Title": "A Licenese to Life","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_027.jpg"</v>
+        <v>{"PuzzleNum": "27","Title": "A Licenese to Life","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_027.jpg"},</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2429,11 +2429,11 @@
         <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "28","Title": "Donuts n' Coffee","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_028.jpg"</v>
+        <v>{"PuzzleNum": "28","Title": "Donuts n' Coffee","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_028.jpg"},</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2453,11 +2453,11 @@
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "29","Title": "Pencil Pushers","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_029.jpg"</v>
+        <v>{"PuzzleNum": "29","Title": "Pencil Pushers","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_029.jpg"},</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2477,11 +2477,11 @@
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "30","Title": "Christmas Creations","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_030.jpg"</v>
+        <v>{"PuzzleNum": "30","Title": "Christmas Creations","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_030.jpg"},</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2501,11 +2501,11 @@
         <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "31","Title": "Winters Wish","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_031.jpg"</v>
+        <v>{"PuzzleNum": "31","Title": "Winters Wish","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_031.jpg"},</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2525,11 +2525,11 @@
         <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "32","Title": "Delightful Donuts","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_032.jpg"</v>
+        <v>{"PuzzleNum": "32","Title": "Delightful Donuts","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_032.jpg"},</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2549,11 +2549,11 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "33","Title": "Succulents","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_033.jpg"</v>
+        <v>{"PuzzleNum": "33","Title": "Succulents","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_033.jpg"},</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2573,11 +2573,11 @@
         <v>7</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>410</v>
+        <v>300</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "34","Title": "Sushi","Pieces": "550","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_034.jpeg"</v>
+        <v>{"PuzzleNum": "34","Title": "Sushi","Pieces": "550","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_034.jpeg"},</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2597,11 +2597,11 @@
         <v>59</v>
       </c>
       <c r="F36" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "35","Title": "Bon Appetit","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_035.jpg"</v>
+        <v>{"PuzzleNum": "35","Title": "Bon Appetit","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_035.jpg"},</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2621,11 +2621,11 @@
         <v>59</v>
       </c>
       <c r="F37" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "36","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_036.jpg"</v>
+        <v>{"PuzzleNum": "36","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_036.jpg"},</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2645,11 +2645,11 @@
         <v>62</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>411</v>
+        <v>303</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "37","Title": "Root Beer at the Butterfields","Pieces": "300","Company": "Buffalo","Size": "21.5 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_037.jpeg"</v>
+        <v>{"PuzzleNum": "37","Title": "Root Beer at the Butterfields","Pieces": "300","Company": "Buffalo","Size": "21.5 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_037.jpeg"},</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2669,11 +2669,11 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "38","Title": "Donut Resist","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_038.jpg"</v>
+        <v>{"PuzzleNum": "38","Title": "Donut Resist","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_038.jpg"},</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2693,11 +2693,11 @@
         <v>59</v>
       </c>
       <c r="F40" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "39","Title": "Este' MacLeod","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_039.jpg"</v>
+        <v>{"PuzzleNum": "39","Title": "Este' MacLeod","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_039.jpg"},</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2717,11 +2717,11 @@
         <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "40","Title": "Mickey and Minnie in Paris","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_040.jpg"</v>
+        <v>{"PuzzleNum": "40","Title": "Mickey and Minnie in Paris","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_040.jpg"},</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2741,11 +2741,11 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "41","Title": "Rainbow Buttons","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_041.jpg"</v>
+        <v>{"PuzzleNum": "41","Title": "Rainbow Buttons","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_041.jpg"},</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2765,11 +2765,11 @@
         <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "42","Title": "Frederick the Literate","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_042.jpg"</v>
+        <v>{"PuzzleNum": "42","Title": "Frederick the Literate","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_042.jpg"},</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2789,11 +2789,11 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "43","Title": "Bobons, Sweets, Dulces","Pieces": "750","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_043.jpg"</v>
+        <v>{"PuzzleNum": "43","Title": "Bobons, Sweets, Dulces","Pieces": "750","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_043.jpg"},</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2813,11 +2813,11 @@
         <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "44","Title": "Seaside","Pieces": "750","Company": "Ceaco","Size": "24 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_044.jpg"</v>
+        <v>{"PuzzleNum": "44","Title": "Seaside","Pieces": "750","Company": "Ceaco","Size": "24 round","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_044.jpg"},</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2837,11 +2837,11 @@
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "45","Title": "Beachcombers","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_045.jpg"</v>
+        <v>{"PuzzleNum": "45","Title": "Beachcombers","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_045.jpg"},</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2861,11 +2861,11 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "46","Title": "Rainbow Marbles","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_046.jpg"</v>
+        <v>{"PuzzleNum": "46","Title": "Rainbow Marbles","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_046.jpg"},</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2885,11 +2885,11 @@
         <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "47","Title": "License Plates","Pieces": "750","Company": "Re-marks","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_047.jpg"</v>
+        <v>{"PuzzleNum": "47","Title": "License Plates","Pieces": "750","Company": "Re-marks","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_047.jpg"},</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2909,11 +2909,11 @@
         <v>34</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "48","Title": "Plumes of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_048.jpg"</v>
+        <v>{"PuzzleNum": "48","Title": "Plumes of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_048.jpg"},</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2933,11 +2933,11 @@
         <v>7</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>412</v>
+        <v>315</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "49","Title": "Autumn Sail","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_049.jpeg"</v>
+        <v>{"PuzzleNum": "49","Title": "Autumn Sail","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_049.jpeg"},</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2957,11 +2957,11 @@
         <v>54</v>
       </c>
       <c r="F51" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "50","Title": "Mandala Stones","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_050.jpg"</v>
+        <v>{"PuzzleNum": "50","Title": "Mandala Stones","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_050.jpg"},</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2981,11 +2981,11 @@
         <v>79</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "51","Title": "Grandiose Greece","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_051.jpg"</v>
+        <v>{"PuzzleNum": "51","Title": "Grandiose Greece","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_051.jpg"},</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -3005,11 +3005,11 @@
         <v>81</v>
       </c>
       <c r="F53" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "52","Title": "Garden Bridge","Pieces": "1000","Company": "Master Pieces","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_052.jpg"</v>
+        <v>{"PuzzleNum": "52","Title": "Garden Bridge","Pieces": "1000","Company": "Master Pieces","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_052.jpg"},</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -3029,11 +3029,11 @@
         <v>34</v>
       </c>
       <c r="F54" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "53","Title": "Drops of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_053.jpg"</v>
+        <v>{"PuzzleNum": "53","Title": "Drops of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_053.jpg"},</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -3053,11 +3053,11 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "54","Title": "Rainbow Clownfish","Pieces": "550","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_054.jpg"</v>
+        <v>{"PuzzleNum": "54","Title": "Rainbow Clownfish","Pieces": "550","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_054.jpg"},</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -3077,11 +3077,11 @@
         <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "55","Title": "Banana Split","Pieces": "1000","Company": "Buffalo","Size": "26.75 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_055.jpg"</v>
+        <v>{"PuzzleNum": "55","Title": "Banana Split","Pieces": "1000","Company": "Buffalo","Size": "26.75 X 19.75","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_055.jpg"},</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -3101,11 +3101,11 @@
         <v>81</v>
       </c>
       <c r="F57" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "56","Title": "Harry Potter Collage","Pieces": "1000","Company": "New York Puzzle Company","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_056.jpg"</v>
+        <v>{"PuzzleNum": "56","Title": "Harry Potter Collage","Pieces": "1000","Company": "New York Puzzle Company","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_056.jpg"},</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -3125,11 +3125,11 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "57","Title": "Happiness Blooms","Pieces": "500","Company": "Lang","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_057.jpg"</v>
+        <v>{"PuzzleNum": "57","Title": "Happiness Blooms","Pieces": "500","Company": "Lang","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_057.jpg"},</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -3149,11 +3149,11 @@
         <v>92</v>
       </c>
       <c r="F59" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "58","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_058.jpg"</v>
+        <v>{"PuzzleNum": "58","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_058.jpg"},</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -3173,11 +3173,11 @@
         <v>79</v>
       </c>
       <c r="F60" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "59","Title": "Escape Puzzle","Pieces": "759","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_059.jpg"</v>
+        <v>{"PuzzleNum": "59","Title": "Escape Puzzle","Pieces": "759","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_059.jpg"},</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -3197,11 +3197,11 @@
         <v>95</v>
       </c>
       <c r="F61" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "60","Title": "Icing on the Cake","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_060.jpg"</v>
+        <v>{"PuzzleNum": "60","Title": "Icing on the Cake","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_060.jpg"},</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -3221,11 +3221,11 @@
         <v>16</v>
       </c>
       <c r="F62" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "61","Title": "Harvest Festival","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_061.jpg"</v>
+        <v>{"PuzzleNum": "61","Title": "Harvest Festival","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_061.jpg"},</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -3245,11 +3245,11 @@
         <v>16</v>
       </c>
       <c r="F63" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "62","Title": "Ski Park City","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_062.jpg"</v>
+        <v>{"PuzzleNum": "62","Title": "Ski Park City","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_062.jpg"},</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -3269,11 +3269,11 @@
         <v>16</v>
       </c>
       <c r="F64" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "63","Title": "Three Little Pigs","Pieces": "100","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_063.jpg"</v>
+        <v>{"PuzzleNum": "63","Title": "Three Little Pigs","Pieces": "100","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_063.jpg"},</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -3293,11 +3293,11 @@
         <v>102</v>
       </c>
       <c r="F65" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "64","Title": "Ice Cream Dream","Pieces": "1000","Company": "Chronicle Books","Size": "25 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_064.jpg"</v>
+        <v>{"PuzzleNum": "64","Title": "Ice Cream Dream","Pieces": "1000","Company": "Chronicle Books","Size": "25 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_064.jpg"},</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -3317,11 +3317,11 @@
         <v>104</v>
       </c>
       <c r="F66" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "65","Title": "Marvel","Pieces": "1000","Company": "Aquarius","Size": "20 X 28","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_065.jpg"</v>
+        <v>{"PuzzleNum": "65","Title": "Marvel","Pieces": "1000","Company": "Aquarius","Size": "20 X 28","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_065.jpg"},</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -3341,11 +3341,11 @@
         <v>95</v>
       </c>
       <c r="F67" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G130" si="1">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F67&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "66","Title": "Feathered Friends","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_066.jpg"</v>
+        <f t="shared" ref="G67:G130" si="1">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F67&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "66","Title": "Feathered Friends","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_066.jpg"},</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -3365,11 +3365,11 @@
         <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "67","Title": "Board Games","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_067.jpg"</v>
+        <v>{"PuzzleNum": "67","Title": "Board Games","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_067.jpg"},</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3389,11 +3389,11 @@
         <v>10</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>413</v>
+        <v>334</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "68","Title": "Cookies &amp; Christmas","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_068.jpeg"</v>
+        <v>{"PuzzleNum": "68","Title": "Cookies &amp; Christmas","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_068.jpeg"},</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3413,11 +3413,11 @@
         <v>95</v>
       </c>
       <c r="F70" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "69","Title": "Cupcakes","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_069.jpg"</v>
+        <v>{"PuzzleNum": "69","Title": "Cupcakes","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_069.jpg"},</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3437,11 +3437,11 @@
         <v>111</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>414</v>
+        <v>336</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "70","Title": "Ship Portal","Pieces": "100","Company": "Great American Puzzle Factory","Size": "13 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_070.jpeg"</v>
+        <v>{"PuzzleNum": "70","Title": "Ship Portal","Pieces": "100","Company": "Great American Puzzle Factory","Size": "13 round","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_070.jpeg"},</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3461,11 +3461,11 @@
         <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "71","Title": "Minnesota Nice up North","Pieces": "550","Company": "Puzzles that Rock","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_071.jpg"</v>
+        <v>{"PuzzleNum": "71","Title": "Minnesota Nice up North","Pieces": "550","Company": "Puzzles that Rock","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_071.jpg"},</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3485,11 +3485,11 @@
         <v>7</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>415</v>
+        <v>338</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "72","Title": "Lake Superior Agates","Pieces": "550","Company": "Erickson Post","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_072.jpeg"</v>
+        <v>{"PuzzleNum": "72","Title": "Lake Superior Agates","Pieces": "550","Company": "Erickson Post","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_072.jpeg"},</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3509,11 +3509,11 @@
         <v>79</v>
       </c>
       <c r="F74" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "73","Title": "Vintage Library","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_073.jpg"</v>
+        <v>{"PuzzleNum": "73","Title": "Vintage Library","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_073.jpg"},</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3533,11 +3533,11 @@
         <v>7</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>416</v>
+        <v>340</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "74","Title": "Butterflies Rock Puddingstone Perch","Pieces": "550","Company": "Puzzle that Rock","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_074.jpeg"</v>
+        <v>{"PuzzleNum": "74","Title": "Butterflies Rock Puddingstone Perch","Pieces": "550","Company": "Puzzle that Rock","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_074.jpeg"},</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3557,11 +3557,11 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "75","Title": "Sea Horsing Around","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_075.jpg"</v>
+        <v>{"PuzzleNum": "75","Title": "Sea Horsing Around","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_075.jpg"},</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3581,11 +3581,11 @@
         <v>121</v>
       </c>
       <c r="F77" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "76","Title": "Grandma's Cookies","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_076.jpg"</v>
+        <v>{"PuzzleNum": "76","Title": "Grandma's Cookies","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_076.jpg"},</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3605,11 +3605,11 @@
         <v>79</v>
       </c>
       <c r="F78" t="s">
-        <v>317</v>
+        <v>343</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "77","Title": "Chocolate Overload","Pieces": "300","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_077.jpg"</v>
+        <v>{"PuzzleNum": "77","Title": "Chocolate Overload","Pieces": "300","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_077.jpg"},</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3629,11 +3629,11 @@
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "78","Title": "Doggie Delight","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_078.jpg"</v>
+        <v>{"PuzzleNum": "78","Title": "Doggie Delight","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_078.jpg"},</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3653,11 +3653,11 @@
         <v>125</v>
       </c>
       <c r="F80" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "79","Title": "Beautiful Horses","Pieces": "200","Company": "Ravensburger","Size": "14.25 X 19.3","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_079.jpg"</v>
+        <v>{"PuzzleNum": "79","Title": "Beautiful Horses","Pieces": "200","Company": "Ravensburger","Size": "14.25 X 19.3","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_079.jpg"},</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3677,11 +3677,11 @@
         <v>81</v>
       </c>
       <c r="F81" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "80","Title": "The Fishing Cabin","Pieces": "1000","Company": "Eurographics","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_080.jpg"</v>
+        <v>{"PuzzleNum": "80","Title": "The Fishing Cabin","Pieces": "1000","Company": "Eurographics","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_080.jpg"},</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3701,11 +3701,11 @@
         <v>130</v>
       </c>
       <c r="F82" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "81","Title": "Peace and Joy","Pieces": "1000","Company": "Go! Games","Size": "19.6 X 29.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_081.jpg"</v>
+        <v>{"PuzzleNum": "81","Title": "Peace and Joy","Pieces": "1000","Company": "Go! Games","Size": "19.6 X 29.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_081.jpg"},</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3725,11 +3725,11 @@
         <v>132</v>
       </c>
       <c r="F83" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "82","Title": "Horse Dream","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_082.jpg"</v>
+        <v>{"PuzzleNum": "82","Title": "Horse Dream","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_082.jpg"},</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3749,11 +3749,11 @@
         <v>132</v>
       </c>
       <c r="F84" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "83","Title": "WIld Jungle","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_083.jpg"</v>
+        <v>{"PuzzleNum": "83","Title": "WIld Jungle","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_083.jpg"},</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3773,11 +3773,11 @@
         <v>132</v>
       </c>
       <c r="F85" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "84","Title": "The Solar System","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_084.jpg"</v>
+        <v>{"PuzzleNum": "84","Title": "The Solar System","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_084.jpg"},</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3797,11 +3797,11 @@
         <v>132</v>
       </c>
       <c r="F86" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "85","Title": "The Christmas Fair","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_085.jpg"</v>
+        <v>{"PuzzleNum": "85","Title": "The Christmas Fair","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_085.jpg"},</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3821,11 +3821,11 @@
         <v>132</v>
       </c>
       <c r="F87" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "86","Title": "The Imaginaries","Pieces": "300","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_086.jpg"</v>
+        <v>{"PuzzleNum": "86","Title": "The Imaginaries","Pieces": "300","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_086.jpg"},</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3845,11 +3845,11 @@
         <v>138</v>
       </c>
       <c r="F88" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "87","Title": "Sweet Tooth","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_087.jpg"</v>
+        <v>{"PuzzleNum": "87","Title": "Sweet Tooth","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_087.jpg"},</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3869,11 +3869,11 @@
         <v>140</v>
       </c>
       <c r="F89" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "88","Title": "Go Fly a Kite","Pieces": "380","Company": "Ravensburger","Size": "26.6 X 10.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_088.jpg"</v>
+        <v>{"PuzzleNum": "88","Title": "Go Fly a Kite","Pieces": "380","Company": "Ravensburger","Size": "26.6 X 10.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_088.jpg"},</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3893,11 +3893,11 @@
         <v>26</v>
       </c>
       <c r="F90" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "89","Title": "MN Abbey Road","Pieces": "500","Company": "Maynards","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_089.jpg"</v>
+        <v>{"PuzzleNum": "89","Title": "MN Abbey Road","Pieces": "500","Company": "Maynards","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_089.jpg"},</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3917,11 +3917,11 @@
         <v>144</v>
       </c>
       <c r="F91" t="s">
-        <v>330</v>
+        <v>356</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "90","Title": "Song for the Season","Pieces": "500","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_090.jpg"</v>
+        <v>{"PuzzleNum": "90","Title": "Song for the Season","Pieces": "500","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_090.jpg"},</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3941,11 +3941,11 @@
         <v>7</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>417</v>
+        <v>357</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "91","Title": "Father's Day Ties","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_091.jpeg"</v>
+        <v>{"PuzzleNum": "91","Title": "Father's Day Ties","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_091.jpeg"},</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3965,11 +3965,11 @@
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "92","Title": "Welcome to My Garden","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_092.jpg"</v>
+        <v>{"PuzzleNum": "92","Title": "Welcome to My Garden","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_092.jpg"},</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3989,11 +3989,11 @@
         <v>148</v>
       </c>
       <c r="F94" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "93","Title": "Love, Home, Family, Friends","Pieces": "400","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_093.jpg"</v>
+        <v>{"PuzzleNum": "93","Title": "Love, Home, Family, Friends","Pieces": "400","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_093.jpg"},</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -4013,11 +4013,11 @@
         <v>79</v>
       </c>
       <c r="F95" t="s">
-        <v>333</v>
+        <v>360</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "94","Title": "Autumn Birds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_094.jpg"</v>
+        <v>{"PuzzleNum": "94","Title": "Autumn Birds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_094.jpg"},</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -4037,11 +4037,11 @@
         <v>79</v>
       </c>
       <c r="F96" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "95","Title": "Drive-thru Route 66","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_095.jpg"</v>
+        <v>{"PuzzleNum": "95","Title": "Drive-thru Route 66","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_095.jpg"},</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -4061,11 +4061,11 @@
         <v>79</v>
       </c>
       <c r="F97" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "96","Title": "Weekend Escape","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_096.jpg"</v>
+        <v>{"PuzzleNum": "96","Title": "Weekend Escape","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_096.jpg"},</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -4085,11 +4085,11 @@
         <v>79</v>
       </c>
       <c r="F98" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "97","Title": "Underwater Smiles","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_097.jpg"</v>
+        <v>{"PuzzleNum": "97","Title": "Underwater Smiles","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_097.jpg"},</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -4109,11 +4109,11 @@
         <v>155</v>
       </c>
       <c r="F99" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "98","Title": "Minnesota Spirit","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_098.jpg"</v>
+        <v>{"PuzzleNum": "98","Title": "Minnesota Spirit","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_098.jpg"},</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -4133,11 +4133,11 @@
         <v>121</v>
       </c>
       <c r="F100" t="s">
-        <v>338</v>
+        <v>365</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "99","Title": "State Plates","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_099.jpg"</v>
+        <v>{"PuzzleNum": "99","Title": "State Plates","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_099.jpg"},</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -4157,11 +4157,11 @@
         <v>155</v>
       </c>
       <c r="F101" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "100","Title": "Cabin Rules","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_100.jpg"</v>
+        <v>{"PuzzleNum": "100","Title": "Cabin Rules","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_100.jpg"},</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -4181,11 +4181,11 @@
         <v>160</v>
       </c>
       <c r="F102" t="s">
-        <v>340</v>
+        <v>367</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "101","Title": "Boat Parade","Pieces": "1000","Company": "Spilsbury Puzzle Co","Size": "26.75 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_101.jpg"</v>
+        <v>{"PuzzleNum": "101","Title": "Boat Parade","Pieces": "1000","Company": "Spilsbury Puzzle Co","Size": "26.75 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_101.jpg"},</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -4205,11 +4205,11 @@
         <v>162</v>
       </c>
       <c r="F103" t="s">
-        <v>341</v>
+        <v>368</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "102","Title": "A Rainbow in Bloom","Pieces": "70","Company": "Springbok","Size": "7 X 7 (Qty 6)","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_102.jpg"</v>
+        <v>{"PuzzleNum": "102","Title": "A Rainbow in Bloom","Pieces": "70","Company": "Springbok","Size": "7 X 7 (Qty 6)","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_102.jpg"},</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4229,11 +4229,11 @@
         <v>138</v>
       </c>
       <c r="F104" t="s">
-        <v>342</v>
+        <v>369</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "103","Title": "Candy Galore","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_103.jpg"</v>
+        <v>{"PuzzleNum": "103","Title": "Candy Galore","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_103.jpg"},</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -4253,11 +4253,11 @@
         <v>144</v>
       </c>
       <c r="F105" t="s">
-        <v>343</v>
+        <v>370</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "104","Title": "Ugly Christmas Sweaters","Pieces": "1000","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_104.jpg"</v>
+        <v>{"PuzzleNum": "104","Title": "Ugly Christmas Sweaters","Pieces": "1000","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_104.jpg"},</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -4277,11 +4277,11 @@
         <v>79</v>
       </c>
       <c r="F106" t="s">
-        <v>344</v>
+        <v>371</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "105","Title": "The Artist's Desk","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_105.jpg"</v>
+        <v>{"PuzzleNum": "105","Title": "The Artist's Desk","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_105.jpg"},</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -4301,11 +4301,11 @@
         <v>79</v>
       </c>
       <c r="F107" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "106","Title": "Disney Pixar Movies","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_106.jpg"</v>
+        <v>{"PuzzleNum": "106","Title": "Disney Pixar Movies","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_106.jpg"},</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -4325,11 +4325,11 @@
         <v>168</v>
       </c>
       <c r="F108" t="s">
-        <v>346</v>
+        <v>373</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "107","Title": "Scorceror's Apprentice","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_107.jpg"</v>
+        <v>{"PuzzleNum": "107","Title": "Scorceror's Apprentice","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_107.jpg"},</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -4349,11 +4349,11 @@
         <v>7</v>
       </c>
       <c r="F109" t="s">
-        <v>347</v>
+        <v>374</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "108","Title": "Disney Chefs","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_108.jpg"</v>
+        <v>{"PuzzleNum": "108","Title": "Disney Chefs","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_108.jpg"},</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -4373,11 +4373,11 @@
         <v>168</v>
       </c>
       <c r="F110" t="s">
-        <v>348</v>
+        <v>375</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_109.jpg"</v>
+        <v>{"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_109.jpg"},</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -4397,11 +4397,11 @@
         <v>172</v>
       </c>
       <c r="F111" t="s">
-        <v>349</v>
+        <v>376</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "110","Title": "Sitting Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_110.jpg"</v>
+        <v>{"PuzzleNum": "110","Title": "Sitting Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_110.jpg"},</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -4421,11 +4421,11 @@
         <v>172</v>
       </c>
       <c r="F112" t="s">
-        <v>350</v>
+        <v>377</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "111","Title": "Danicing Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_111.jpg"</v>
+        <v>{"PuzzleNum": "111","Title": "Danicing Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_111.jpg"},</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -4445,11 +4445,11 @@
         <v>176</v>
       </c>
       <c r="F113" t="s">
-        <v>351</v>
+        <v>378</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_112.jpg"</v>
+        <v>{"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_112.jpg"},</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -4469,11 +4469,11 @@
         <v>92</v>
       </c>
       <c r="F114" t="s">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_113.jpg"</v>
+        <v>{"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_113.jpg"},</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -4493,11 +4493,11 @@
         <v>179</v>
       </c>
       <c r="F115" t="s">
-        <v>353</v>
+        <v>380</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_114.jpg"</v>
+        <v>{"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_114.jpg"},</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -4517,11 +4517,11 @@
         <v>92</v>
       </c>
       <c r="F116" t="s">
-        <v>354</v>
+        <v>381</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_115.jpg"</v>
+        <v>{"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_115.jpg"},</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -4541,11 +4541,11 @@
         <v>92</v>
       </c>
       <c r="F117" t="s">
-        <v>355</v>
+        <v>382</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_116.jpg"</v>
+        <v>{"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_116.jpg"},</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -4565,11 +4565,11 @@
         <v>176</v>
       </c>
       <c r="F118" t="s">
-        <v>356</v>
+        <v>383</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_117.jpg"</v>
+        <v>{"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_117.jpg"},</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -4589,11 +4589,11 @@
         <v>92</v>
       </c>
       <c r="F119" t="s">
-        <v>357</v>
+        <v>384</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_118.jpg"</v>
+        <v>{"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_118.jpg"},</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4610,11 +4610,11 @@
         <v>185</v>
       </c>
       <c r="F120" t="s">
-        <v>358</v>
+        <v>385</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "119","Title": "Unknown","Pieces": "1000","Company": "unknown","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_119.jpg"</v>
+        <v>{"PuzzleNum": "119","Title": "Unknown","Pieces": "1000","Company": "unknown","Size": "","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_119.jpg"},</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -4634,11 +4634,11 @@
         <v>187</v>
       </c>
       <c r="F121" t="s">
-        <v>359</v>
+        <v>386</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "120","Title": "Family Vacation","Pieces": "2000","Company": "Buffalo","Size": "38.5 X 26.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_120.jpg"</v>
+        <v>{"PuzzleNum": "120","Title": "Family Vacation","Pieces": "2000","Company": "Buffalo","Size": "38.5 X 26.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_120.jpg"},</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4658,11 +4658,11 @@
         <v>121</v>
       </c>
       <c r="F122" t="s">
-        <v>360</v>
+        <v>387</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "121","Title": "Ideal Bookshelf","Pieces": "1000","Company": "Galison","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_121.jpg"</v>
+        <v>{"PuzzleNum": "121","Title": "Ideal Bookshelf","Pieces": "1000","Company": "Galison","Size": "27 X 20.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_121.jpg"},</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4682,11 +4682,11 @@
         <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>361</v>
+        <v>388</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "122","Title": "Singbird Serenade","Pieces": "500","Company": "Puzzle Twist","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_122.jpg"</v>
+        <v>{"PuzzleNum": "122","Title": "Singbird Serenade","Pieces": "500","Company": "Puzzle Twist","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_122.jpg"},</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -4706,11 +4706,11 @@
         <v>41</v>
       </c>
       <c r="F124" t="s">
-        <v>251</v>
+        <v>389</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "123","Title": "Underwater Seascape","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_123.jpg"</v>
+        <v>{"PuzzleNum": "123","Title": "Underwater Seascape","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_123.jpg"},</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4730,11 +4730,11 @@
         <v>193</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>362</v>
+        <v>390</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "124","Title": "The Flintstones","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_124.jpg"</v>
+        <v>{"PuzzleNum": "124","Title": "The Flintstones","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_124.jpg"},</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -4754,11 +4754,11 @@
         <v>193</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "125","Title": "Scooby-Doo!","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_125.jpg"</v>
+        <v>{"PuzzleNum": "125","Title": "Scooby-Doo!","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_125.jpg"},</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -4778,11 +4778,11 @@
         <v>193</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>364</v>
+        <v>392</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "126","Title": "The Jetsons","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_126.jpg"</v>
+        <v>{"PuzzleNum": "126","Title": "The Jetsons","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_126.jpg"},</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -4802,11 +4802,11 @@
         <v>34</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "127","Title": "Morning Magic","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_127.jpg"</v>
+        <v>{"PuzzleNum": "127","Title": "Morning Magic","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_127.jpg"},</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4826,11 +4826,11 @@
         <v>199</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>366</v>
+        <v>394</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "128","Title": "Circle of Colors: Animals","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_128.jpg"</v>
+        <v>{"PuzzleNum": "128","Title": "Circle of Colors: Animals","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_128.jpg"},</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -4850,11 +4850,11 @@
         <v>79</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>367</v>
+        <v>395</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_129.jpg"</v>
+        <v>{"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_129.jpg"},</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -4874,11 +4874,11 @@
         <v>7</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>368</v>
+        <v>396</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" ref="G131:G176" si="2">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F131&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "130","Title": "Animal Yoga","Pieces": "500","Company": "unknown","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_130.jpg"</v>
+        <f t="shared" ref="G131:G176" si="2">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F131&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "130","Title": "Animal Yoga","Pieces": "500","Company": "unknown","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_130.jpg"},</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -4898,11 +4898,11 @@
         <v>79</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>369</v>
+        <v>397</v>
       </c>
       <c r="G132" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "131","Title": "Christmas Singbirds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_131.jpg"</v>
+        <v>{"PuzzleNum": "131","Title": "Christmas Singbirds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_131.jpg"},</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -4922,11 +4922,11 @@
         <v>132</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>370</v>
+        <v>398</v>
       </c>
       <c r="G133" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "132","Title": "Typefaces","Pieces": "500","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_132.jpg"</v>
+        <v>{"PuzzleNum": "132","Title": "Typefaces","Pieces": "500","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_132.jpg"},</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -4946,11 +4946,11 @@
         <v>26</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="G134" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "133","Title": "Tree of Life","Pieces": "275","Company": "Cobble Hill","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_133.jpg"</v>
+        <v>{"PuzzleNum": "133","Title": "Tree of Life","Pieces": "275","Company": "Cobble Hill","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_133.jpg"},</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -4970,11 +4970,11 @@
         <v>26</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>372</v>
+        <v>400</v>
       </c>
       <c r="G135" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "134","Title": "MinneSNOWta","Pieces": "500","Company": "PuzzleTwist","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_134.jpg"</v>
+        <v>{"PuzzleNum": "134","Title": "MinneSNOWta","Pieces": "500","Company": "PuzzleTwist","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_134.jpg"},</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -4994,11 +4994,11 @@
         <v>7</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="G136" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "135","Title": "Up","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_135.jpg"</v>
+        <v>{"PuzzleNum": "135","Title": "Up","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_135.jpg"},</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -5018,11 +5018,11 @@
         <v>26</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="G137" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "136","Title": "San Diego Zoo","Pieces": "500","Company": "San Diego Zoo Wildlife Alliance","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_136.jpg"</v>
+        <v>{"PuzzleNum": "136","Title": "San Diego Zoo","Pieces": "500","Company": "San Diego Zoo Wildlife Alliance","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_136.jpg"},</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -5042,11 +5042,11 @@
         <v>193</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
       <c r="G138" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "137","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_137.jpg"</v>
+        <v>{"PuzzleNum": "137","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "14 X 19","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_137.jpg"},</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -5066,11 +5066,11 @@
         <v>79</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="G139" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "138","Title": "Winnie the Pooh","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_138.jpg"</v>
+        <v>{"PuzzleNum": "138","Title": "Winnie the Pooh","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_138.jpg"},</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -5090,11 +5090,11 @@
         <v>92</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>377</v>
+        <v>405</v>
       </c>
       <c r="G140" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "139","Title": "Scooby Doo Haunted Game","Pieces": "200","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_139.jpg"</v>
+        <v>{"PuzzleNum": "139","Title": "Scooby Doo Haunted Game","Pieces": "200","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_139.jpg"},</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -5114,11 +5114,11 @@
         <v>92</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="G141" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "140","Title": "Toy Story","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_140.jpg"</v>
+        <v>{"PuzzleNum": "140","Title": "Toy Story","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_140.jpg"},</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -5135,11 +5135,11 @@
         <v>215</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="G142" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "141","Title": "Pups in Cups","Pieces": "500 total","Company": "Rose Art","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_141.jpg"</v>
+        <v>{"PuzzleNum": "141","Title": "Pups in Cups","Pieces": "500 total","Company": "Rose Art","Size": "","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_141.jpg"},</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -5159,11 +5159,11 @@
         <v>217</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
       <c r="G143" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "142","Title": "You Betcha!","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_142.jpg"</v>
+        <v>{"PuzzleNum": "142","Title": "You Betcha!","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_142.jpg"},</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -5183,11 +5183,11 @@
         <v>7</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>381</v>
+        <v>409</v>
       </c>
       <c r="G144" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "143","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_143.jpg"</v>
+        <v>{"PuzzleNum": "143","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_143.jpg"},</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -5207,11 +5207,11 @@
         <v>79</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>382</v>
+        <v>410</v>
       </c>
       <c r="G145" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "144","Title": "Goofy","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_144.jpg"</v>
+        <v>{"PuzzleNum": "144","Title": "Goofy","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_144.jpg"},</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -5231,11 +5231,11 @@
         <v>79</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="G146" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "145","Title": "Barbie Around the World","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_145.jpg"</v>
+        <v>{"PuzzleNum": "145","Title": "Barbie Around the World","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_145.jpg"},</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -5255,11 +5255,11 @@
         <v>92</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
       <c r="G147" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "146","Title": "Pooh to the Rescue","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_146.jpg"</v>
+        <v>{"PuzzleNum": "146","Title": "Pooh to the Rescue","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_146.jpg"},</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -5279,11 +5279,11 @@
         <v>223</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>385</v>
+        <v>413</v>
       </c>
       <c r="G148" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_147.jpg"</v>
+        <v>{"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_147.jpg"},</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -5303,11 +5303,11 @@
         <v>7</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>386</v>
+        <v>414</v>
       </c>
       <c r="G149" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "148","Title": "Gnomes Get Baking","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_148.jpg"</v>
+        <v>{"PuzzleNum": "148","Title": "Gnomes Get Baking","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_148.jpg"},</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -5327,11 +5327,11 @@
         <v>7</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>387</v>
+        <v>415</v>
       </c>
       <c r="G150" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "149","Title": "Mickey and Friends","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_149.jpg"</v>
+        <v>{"PuzzleNum": "149","Title": "Mickey and Friends","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_149.jpg"},</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -5351,11 +5351,11 @@
         <v>7</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>388</v>
+        <v>416</v>
       </c>
       <c r="G151" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "150","Title": "Coming Home","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_150.jpg"</v>
+        <v>{"PuzzleNum": "150","Title": "Coming Home","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_150.jpg"},</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -5375,11 +5375,11 @@
         <v>228</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>389</v>
+        <v>417</v>
       </c>
       <c r="G152" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "151","Title": "Sky Roads","Pieces": "1000","Company": "Buffalo","Size": "26.76 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_151.jpg"</v>
+        <v>{"PuzzleNum": "151","Title": "Sky Roads","Pieces": "1000","Company": "Buffalo","Size": "26.76 X 19.75","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_151.jpg"},</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -5399,11 +5399,11 @@
         <v>34</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>390</v>
+        <v>418</v>
       </c>
       <c r="G153" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "152","Title": "Front Porch Flag","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_152.jpg"</v>
+        <v>{"PuzzleNum": "152","Title": "Front Porch Flag","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_152.jpg"},</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -5423,11 +5423,11 @@
         <v>95</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>391</v>
+        <v>419</v>
       </c>
       <c r="G154" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "153","Title": "Springtime Cookies","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_153.jpg"</v>
+        <v>{"PuzzleNum": "153","Title": "Springtime Cookies","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_153.jpg"},</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -5447,11 +5447,11 @@
         <v>79</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>392</v>
+        <v>420</v>
       </c>
       <c r="G155" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "154","Title": "Tom + Jerry Hall of Fame","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_154.jpg"</v>
+        <v>{"PuzzleNum": "154","Title": "Tom + Jerry Hall of Fame","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_154.jpg"},</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -5471,11 +5471,11 @@
         <v>199</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="G156" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "155","Title": "Fruits + Vegetables","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_155.jpg"</v>
+        <v>{"PuzzleNum": "155","Title": "Fruits + Vegetables","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_155.jpg"},</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -5495,11 +5495,11 @@
         <v>234</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>394</v>
+        <v>422</v>
       </c>
       <c r="G157" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "156","Title": "Bedtime Stories","Pieces": "1000","Company": "Re-marks","Size": "19.25 X 26.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_156.jpg"</v>
+        <v>{"PuzzleNum": "156","Title": "Bedtime Stories","Pieces": "1000","Company": "Re-marks","Size": "19.25 X 26.75","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_156.jpg"},</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -5519,11 +5519,11 @@
         <v>34</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>395</v>
+        <v>423</v>
       </c>
       <c r="G158" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "157","Title": "Candy Chrome","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_157.jpg"</v>
+        <v>{"PuzzleNum": "157","Title": "Candy Chrome","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_157.jpg"},</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5543,11 +5543,11 @@
         <v>7</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
       <c r="G159" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "158","Title": "Fireworks Finale","Pieces": "750","Company": "MasterPieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_158.jpg"</v>
+        <v>{"PuzzleNum": "158","Title": "Fireworks Finale","Pieces": "750","Company": "MasterPieces","Size": "24 X 18","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_158.jpg"},</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -5567,11 +5567,11 @@
         <v>217</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
       <c r="G160" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "159","Title": "Horseplay","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_159.jpg"</v>
+        <v>{"PuzzleNum": "159","Title": "Horseplay","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_159.jpg"},</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5591,11 +5591,11 @@
         <v>239</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>398</v>
+        <v>426</v>
       </c>
       <c r="G161" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "160","Title": "Nordic Love","Pieces": "1000","Company": "PuzzleTwist","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_160.jpg"</v>
+        <v>{"PuzzleNum": "160","Title": "Nordic Love","Pieces": "1000","Company": "PuzzleTwist","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_160.jpg"},</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5615,11 +5615,11 @@
         <v>217</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>399</v>
+        <v>427</v>
       </c>
       <c r="G162" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "161","Title": "Hitting the Road","Pieces": "500","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_161.jpg"</v>
+        <v>{"PuzzleNum": "161","Title": "Hitting the Road","Pieces": "500","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_161.jpg"},</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -5639,11 +5639,11 @@
         <v>239</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>400</v>
+        <v>428</v>
       </c>
       <c r="G163" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "162","Title": "VW Gone Places","Pieces": "1000","Company": "Eurographics","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_162.jpg"</v>
+        <v>{"PuzzleNum": "162","Title": "VW Gone Places","Pieces": "1000","Company": "Eurographics","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_162.jpg"},</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5663,11 +5663,11 @@
         <v>244</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>401</v>
+        <v>429</v>
       </c>
       <c r="G164" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "163","Title": "Love at Home","Pieces": "500","Company": "Colorly Love","Size": "16 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_163.jpg"</v>
+        <v>{"PuzzleNum": "163","Title": "Love at Home","Pieces": "500","Company": "Colorly Love","Size": "16 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_163.jpg"},</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5687,11 +5687,11 @@
         <v>246</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>402</v>
+        <v>430</v>
       </c>
       <c r="G165" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "164","Title": "Childhood Stories","Pieces": "400","Company": "Springbok","Size": "20.5 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_164.jpg"</v>
+        <v>{"PuzzleNum": "164","Title": "Childhood Stories","Pieces": "400","Company": "Springbok","Size": "20.5 X 27","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_164.jpg"},</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5711,11 +5711,11 @@
         <v>217</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>403</v>
+        <v>431</v>
       </c>
       <c r="G166" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "165","Title": "Winter Welcome","Pieces": "1000","Company": "Vermont Christmas Company","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_165.jpg"</v>
+        <v>{"PuzzleNum": "165","Title": "Winter Welcome","Pieces": "1000","Company": "Vermont Christmas Company","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_165.jpg"},</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5735,11 +5735,11 @@
         <v>26</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
       <c r="G167" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "166","Title": "Christmas Barn Snowman","Pieces": "500","Company": "Bits and Pieces","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_166.jpg"</v>
+        <v>{"PuzzleNum": "166","Title": "Christmas Barn Snowman","Pieces": "500","Company": "Bits and Pieces","Size": "18 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_166.jpg"},</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5759,11 +5759,11 @@
         <v>217</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>405</v>
+        <v>433</v>
       </c>
       <c r="G168" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "167","Title": "Farmer's Market Trucks","Pieces": "1000","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_167.jpg"</v>
+        <v>{"PuzzleNum": "167","Title": "Farmer's Market Trucks","Pieces": "1000","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_167.jpg"},</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5771,7 +5771,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>419</v>
+        <v>252</v>
       </c>
       <c r="C169">
         <v>500</v>
@@ -5780,14 +5780,14 @@
         <v>18</v>
       </c>
       <c r="E169" t="s">
-        <v>427</v>
+        <v>260</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>434</v>
       </c>
       <c r="G169" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "168","Title": "Sun and Sea","Pieces": "500","Company": "Ravensburger","Size": "27.5 X 19.67","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg"</v>
+        <v>{"PuzzleNum": "168","Title": "Sun and Sea","Pieces": "500","Company": "Ravensburger","Size": "27.5 X 19.67","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_168.jpg"},</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5795,7 +5795,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>420</v>
+        <v>253</v>
       </c>
       <c r="C170">
         <v>500</v>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg"</v>
+        <v>{"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_169.jpg"},</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5819,23 +5819,23 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>421</v>
+        <v>254</v>
       </c>
       <c r="C171">
         <v>1000</v>
       </c>
       <c r="D171" t="s">
-        <v>428</v>
+        <v>261</v>
       </c>
       <c r="E171" t="s">
-        <v>429</v>
+        <v>262</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>436</v>
       </c>
       <c r="G171" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg"</v>
+        <v>{"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_170.jpg"},</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5843,7 +5843,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>422</v>
+        <v>255</v>
       </c>
       <c r="C172">
         <v>500</v>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="G172" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "171","Title": "Jellies &amp; Jams","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg"</v>
+        <v>{"PuzzleNum": "171","Title": "Jellies &amp; Jams","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_171.jpg"},</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5867,13 +5867,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>423</v>
+        <v>256</v>
       </c>
       <c r="C173">
         <v>1000</v>
       </c>
       <c r="D173" t="s">
-        <v>430</v>
+        <v>263</v>
       </c>
       <c r="E173" t="s">
         <v>138</v>
@@ -5883,7 +5883,7 @@
       </c>
       <c r="G173" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "172","Title": "Backyard BBQ","Pieces": "1000","Company": "White Mountain","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_172.jpg"</v>
+        <v>{"PuzzleNum": "172","Title": "Backyard BBQ","Pieces": "1000","Company": "White Mountain","Size": "30 X 24","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_172.jpg"},</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5891,7 +5891,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>424</v>
+        <v>257</v>
       </c>
       <c r="C174">
         <v>1000</v>
@@ -5900,14 +5900,14 @@
         <v>12</v>
       </c>
       <c r="E174" t="s">
-        <v>431</v>
+        <v>264</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>439</v>
       </c>
       <c r="G174" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "173","Title": "Blossoms and Kittens Quilt","Pieces": "1000","Company": "Cobble Hill","Size": "26.625 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_173.jpg"</v>
+        <v>{"PuzzleNum": "173","Title": "Blossoms and Kittens Quilt","Pieces": "1000","Company": "Cobble Hill","Size": "26.625 X 19.25","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_173.jpg"},</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5915,23 +5915,23 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>425</v>
+        <v>258</v>
       </c>
       <c r="C175">
         <v>1000</v>
       </c>
       <c r="D175" t="s">
-        <v>432</v>
+        <v>265</v>
       </c>
       <c r="E175" t="s">
-        <v>433</v>
+        <v>266</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>440</v>
       </c>
       <c r="G175" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "174","Title": "Honey and Tea","Pieces": "1000","Company": "Sunsout","Size": "35 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_174.jpg"</v>
+        <v>{"PuzzleNum": "174","Title": "Honey and Tea","Pieces": "1000","Company": "Sunsout","Size": "35 X 27","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_174.jpg"},</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5939,7 +5939,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>426</v>
+        <v>259</v>
       </c>
       <c r="C176">
         <v>1000</v>
@@ -5955,77 +5955,77 @@
       </c>
       <c r="G176" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "175","Title": "Christmas Carolers","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg"</v>
+        <v>{"PuzzleNum": "175","Title": "Christmas Carolers","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/DALeske.github.io/tree/main/static/images/Puzzle_175.jpg"},</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E124" xr:uid="{4443A7F1-90C3-4D7D-8B82-1D6A6D8DE156}"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{571D22FC-DB88-4FB8-8013-C11BC25C5B79}"/>
-    <hyperlink ref="F125" r:id="rId2" xr:uid="{C38A8CF9-921C-41A9-9750-98468B86A600}"/>
-    <hyperlink ref="F126" r:id="rId3" xr:uid="{E28CBC53-67CB-4F10-8A3F-02516FBB80F5}"/>
-    <hyperlink ref="F127" r:id="rId4" xr:uid="{830D4D20-F027-4A84-98C2-CD0FFED0CDB5}"/>
-    <hyperlink ref="F128" r:id="rId5" xr:uid="{49145DCD-4245-425F-96BA-98FB48E33EC5}"/>
-    <hyperlink ref="F129" r:id="rId6" xr:uid="{C3114097-3B1A-4A28-B215-D64D8DBD1167}"/>
-    <hyperlink ref="F130" r:id="rId7" xr:uid="{E3193E45-8BB0-4334-8DFD-08E0E7DAC7C2}"/>
-    <hyperlink ref="F131" r:id="rId8" xr:uid="{CA51AE1B-389E-48A3-B1E5-E664AD8E0C70}"/>
-    <hyperlink ref="F132" r:id="rId9" xr:uid="{60AAA66E-E32B-4357-B41F-BBCDB4C5EAD3}"/>
-    <hyperlink ref="F133" r:id="rId10" xr:uid="{B6F2262C-DB6D-4DFE-939F-F2C496FD3731}"/>
-    <hyperlink ref="F134" r:id="rId11" xr:uid="{02F679E2-6CA6-465F-B708-BD4B5B0E5D57}"/>
-    <hyperlink ref="F135" r:id="rId12" xr:uid="{EC01A0A5-DDA8-42EE-89BE-19554945B928}"/>
-    <hyperlink ref="F136" r:id="rId13" xr:uid="{8004C009-D194-48E4-92C7-C99780C9B6E1}"/>
-    <hyperlink ref="F137" r:id="rId14" xr:uid="{BFF09ED8-842B-4512-AA1C-147BC8F456FF}"/>
-    <hyperlink ref="F138" r:id="rId15" xr:uid="{72803A25-C66D-44B6-87E1-40744E909890}"/>
-    <hyperlink ref="F139" r:id="rId16" xr:uid="{AE641D10-0A3E-4BD6-A69C-E9848ED93061}"/>
-    <hyperlink ref="F140" r:id="rId17" xr:uid="{3B381371-1139-4C0C-A787-2EC9397516BF}"/>
-    <hyperlink ref="F141" r:id="rId18" xr:uid="{D578CB73-FD33-4A3D-9CBE-92B9AC61F540}"/>
-    <hyperlink ref="F142" r:id="rId19" xr:uid="{8680E53F-4A34-4168-9EFC-B27D8EB6E66C}"/>
-    <hyperlink ref="F143" r:id="rId20" xr:uid="{19863001-FCB3-4A77-90DA-3E2009851B61}"/>
-    <hyperlink ref="F144" r:id="rId21" xr:uid="{98D74388-ED21-4467-86DD-408FAA40B5B4}"/>
-    <hyperlink ref="F145" r:id="rId22" xr:uid="{A518F626-0C90-4241-9BEC-03970993627C}"/>
-    <hyperlink ref="F146" r:id="rId23" xr:uid="{405A4C88-0828-4299-9CDD-BDD630C21311}"/>
-    <hyperlink ref="F147" r:id="rId24" xr:uid="{DA38291B-FFAD-4DC8-A23A-C3B99F356BE7}"/>
-    <hyperlink ref="F148" r:id="rId25" xr:uid="{C2A456ED-6D5B-4C3E-9844-193D4D7BF02D}"/>
-    <hyperlink ref="F149" r:id="rId26" xr:uid="{B5981099-B506-40F1-B2E6-599B08ECFB7F}"/>
-    <hyperlink ref="F150" r:id="rId27" xr:uid="{BF31C8D8-8A6E-4AB0-83A4-3295AB77C2A1}"/>
-    <hyperlink ref="F151" r:id="rId28" xr:uid="{6C0CF121-70D6-4779-9E7B-E5AC881AE1F4}"/>
-    <hyperlink ref="F152" r:id="rId29" xr:uid="{B555475D-AA5D-4DD7-BD86-425121D0B585}"/>
-    <hyperlink ref="F153" r:id="rId30" xr:uid="{59655042-3D0F-4988-AF94-D2EAE837D9F1}"/>
-    <hyperlink ref="F154" r:id="rId31" xr:uid="{B65B57F5-DDDC-421B-86CB-AA7B9EC83EA4}"/>
-    <hyperlink ref="F155" r:id="rId32" xr:uid="{F7E73982-80D6-4ADD-81F1-C87F2F1A6052}"/>
-    <hyperlink ref="F156" r:id="rId33" xr:uid="{486B1A09-D1FF-4A76-8065-DAF5622FEE85}"/>
-    <hyperlink ref="F157" r:id="rId34" xr:uid="{27D8A5BE-EAB4-4EA1-A209-A799E4972A33}"/>
-    <hyperlink ref="F158" r:id="rId35" xr:uid="{3DED97D7-548F-43C5-AFEB-0E42878C7F16}"/>
-    <hyperlink ref="F159" r:id="rId36" xr:uid="{C40836AF-253B-4968-A180-3D778F4B000D}"/>
-    <hyperlink ref="F160" r:id="rId37" xr:uid="{70760C64-1062-467B-B493-B3D18A67C06D}"/>
-    <hyperlink ref="F161" r:id="rId38" xr:uid="{1751117D-F718-42AA-8EEF-C314BD4E6EDD}"/>
-    <hyperlink ref="F162" r:id="rId39" xr:uid="{C2D46308-E84C-4EB6-A2A7-F0CD5644B86A}"/>
-    <hyperlink ref="F163" r:id="rId40" xr:uid="{D9E751C4-57E6-4426-AD5B-E8E35CA711A8}"/>
-    <hyperlink ref="F164" r:id="rId41" xr:uid="{1E3090DE-5F14-40A0-B068-FA0410047228}"/>
-    <hyperlink ref="F165" r:id="rId42" xr:uid="{000BA945-168D-4514-BA43-5983EFFE571D}"/>
-    <hyperlink ref="F166" r:id="rId43" xr:uid="{41C1DC10-A3EB-4671-A787-A8B6D8D6C4E6}"/>
-    <hyperlink ref="F167" r:id="rId44" xr:uid="{A0DED850-9723-4A31-BAD8-4CCDD469CE9D}"/>
-    <hyperlink ref="F168" r:id="rId45" xr:uid="{BADB420B-5F67-48A7-901E-9D9F0A85E49A}"/>
-    <hyperlink ref="F2" r:id="rId46" xr:uid="{D43A0608-3025-4E10-8E2E-5311FC61D4B4}"/>
-    <hyperlink ref="F7" r:id="rId47" xr:uid="{076A97D8-03AD-4176-9564-55FABF74946B}"/>
-    <hyperlink ref="F11" r:id="rId48" xr:uid="{AA7039FA-CD6C-4742-8C77-40090A0B41D6}"/>
-    <hyperlink ref="F13" r:id="rId49" xr:uid="{13F311E4-36BA-4CFD-998B-C1E9EDAEDD6C}"/>
-    <hyperlink ref="F35" r:id="rId50" xr:uid="{BA484B96-6FE5-4E91-A6B9-A3AE8C72FABE}"/>
-    <hyperlink ref="F38" r:id="rId51" xr:uid="{6B26CD61-05BD-4FBE-99EA-69638465E280}"/>
-    <hyperlink ref="F50" r:id="rId52" xr:uid="{28E0AAFD-810A-4D4B-808B-C26BE5C7FDF9}"/>
-    <hyperlink ref="F69" r:id="rId53" xr:uid="{14C00680-EB91-4078-A7EB-7CDD767B6010}"/>
-    <hyperlink ref="F71" r:id="rId54" xr:uid="{C6DF508C-65F2-4339-85EE-0627C6CB9023}"/>
-    <hyperlink ref="F73" r:id="rId55" xr:uid="{D349BC95-A2D9-41A1-85BC-A99C7E9055CE}"/>
-    <hyperlink ref="F75" r:id="rId56" xr:uid="{6A58F0CE-BA52-47BB-A249-7C0BC00EDCCC}"/>
-    <hyperlink ref="F92" r:id="rId57" xr:uid="{B70BF618-8F37-4856-B7C7-2DD4686C8938}"/>
-    <hyperlink ref="F169" r:id="rId58" xr:uid="{72875193-4BB9-4298-B334-D45C032E669B}"/>
-    <hyperlink ref="F170" r:id="rId59" xr:uid="{7CFC5301-A5E3-4A5D-97C6-A4C0EE0406AE}"/>
-    <hyperlink ref="F171" r:id="rId60" xr:uid="{D4992F6F-89C9-4647-94B6-6C8589D74789}"/>
-    <hyperlink ref="F172" r:id="rId61" xr:uid="{3ED0D14C-F5A3-4C07-873B-BDA1D1C0A1D6}"/>
-    <hyperlink ref="F173" r:id="rId62" xr:uid="{8DD6AC65-41C0-4879-835C-BBF947A1FED4}"/>
-    <hyperlink ref="F174" r:id="rId63" xr:uid="{65D2A0A5-63D9-4E7C-92FA-A797E8CB9E28}"/>
-    <hyperlink ref="F175" r:id="rId64" xr:uid="{8A4ADCD1-3C0B-4AFF-8BAF-237C74CC9224}"/>
-    <hyperlink ref="F176" r:id="rId65" xr:uid="{218C2329-C30A-4A9F-81F1-5E084F34D55D}"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_002.jpg" xr:uid="{571D22FC-DB88-4FB8-8013-C11BC25C5B79}"/>
+    <hyperlink ref="F125" r:id="rId2" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_124.jpg" xr:uid="{C38A8CF9-921C-41A9-9750-98468B86A600}"/>
+    <hyperlink ref="F126" r:id="rId3" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_125.jpg" xr:uid="{E28CBC53-67CB-4F10-8A3F-02516FBB80F5}"/>
+    <hyperlink ref="F127" r:id="rId4" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_126.jpg" xr:uid="{830D4D20-F027-4A84-98C2-CD0FFED0CDB5}"/>
+    <hyperlink ref="F128" r:id="rId5" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_127.jpg" xr:uid="{49145DCD-4245-425F-96BA-98FB48E33EC5}"/>
+    <hyperlink ref="F129" r:id="rId6" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_128.jpg" xr:uid="{C3114097-3B1A-4A28-B215-D64D8DBD1167}"/>
+    <hyperlink ref="F130" r:id="rId7" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_129.jpg" xr:uid="{E3193E45-8BB0-4334-8DFD-08E0E7DAC7C2}"/>
+    <hyperlink ref="F131" r:id="rId8" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_130.jpg" xr:uid="{CA51AE1B-389E-48A3-B1E5-E664AD8E0C70}"/>
+    <hyperlink ref="F132" r:id="rId9" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_131.jpg" xr:uid="{60AAA66E-E32B-4357-B41F-BBCDB4C5EAD3}"/>
+    <hyperlink ref="F133" r:id="rId10" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_132.jpg" xr:uid="{B6F2262C-DB6D-4DFE-939F-F2C496FD3731}"/>
+    <hyperlink ref="F134" r:id="rId11" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_133.jpg" xr:uid="{02F679E2-6CA6-465F-B708-BD4B5B0E5D57}"/>
+    <hyperlink ref="F135" r:id="rId12" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_134.jpg" xr:uid="{EC01A0A5-DDA8-42EE-89BE-19554945B928}"/>
+    <hyperlink ref="F136" r:id="rId13" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_135.jpg" xr:uid="{8004C009-D194-48E4-92C7-C99780C9B6E1}"/>
+    <hyperlink ref="F137" r:id="rId14" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_136.jpg" xr:uid="{BFF09ED8-842B-4512-AA1C-147BC8F456FF}"/>
+    <hyperlink ref="F138" r:id="rId15" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_137.jpg" xr:uid="{72803A25-C66D-44B6-87E1-40744E909890}"/>
+    <hyperlink ref="F139" r:id="rId16" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_138.jpg" xr:uid="{AE641D10-0A3E-4BD6-A69C-E9848ED93061}"/>
+    <hyperlink ref="F140" r:id="rId17" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_139.jpg" xr:uid="{3B381371-1139-4C0C-A787-2EC9397516BF}"/>
+    <hyperlink ref="F141" r:id="rId18" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_140.jpg" xr:uid="{D578CB73-FD33-4A3D-9CBE-92B9AC61F540}"/>
+    <hyperlink ref="F142" r:id="rId19" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_141.jpg" xr:uid="{8680E53F-4A34-4168-9EFC-B27D8EB6E66C}"/>
+    <hyperlink ref="F143" r:id="rId20" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_142.jpg" xr:uid="{19863001-FCB3-4A77-90DA-3E2009851B61}"/>
+    <hyperlink ref="F144" r:id="rId21" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_143.jpg" xr:uid="{98D74388-ED21-4467-86DD-408FAA40B5B4}"/>
+    <hyperlink ref="F145" r:id="rId22" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_144.jpg" xr:uid="{A518F626-0C90-4241-9BEC-03970993627C}"/>
+    <hyperlink ref="F146" r:id="rId23" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_145.jpg" xr:uid="{405A4C88-0828-4299-9CDD-BDD630C21311}"/>
+    <hyperlink ref="F147" r:id="rId24" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_146.jpg" xr:uid="{DA38291B-FFAD-4DC8-A23A-C3B99F356BE7}"/>
+    <hyperlink ref="F148" r:id="rId25" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_147.jpg" xr:uid="{C2A456ED-6D5B-4C3E-9844-193D4D7BF02D}"/>
+    <hyperlink ref="F149" r:id="rId26" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_148.jpg" xr:uid="{B5981099-B506-40F1-B2E6-599B08ECFB7F}"/>
+    <hyperlink ref="F150" r:id="rId27" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_149.jpg" xr:uid="{BF31C8D8-8A6E-4AB0-83A4-3295AB77C2A1}"/>
+    <hyperlink ref="F151" r:id="rId28" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_150.jpg" xr:uid="{6C0CF121-70D6-4779-9E7B-E5AC881AE1F4}"/>
+    <hyperlink ref="F152" r:id="rId29" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_151.jpg" xr:uid="{B555475D-AA5D-4DD7-BD86-425121D0B585}"/>
+    <hyperlink ref="F153" r:id="rId30" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_152.jpg" xr:uid="{59655042-3D0F-4988-AF94-D2EAE837D9F1}"/>
+    <hyperlink ref="F154" r:id="rId31" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_153.jpg" xr:uid="{B65B57F5-DDDC-421B-86CB-AA7B9EC83EA4}"/>
+    <hyperlink ref="F155" r:id="rId32" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_154.jpg" xr:uid="{F7E73982-80D6-4ADD-81F1-C87F2F1A6052}"/>
+    <hyperlink ref="F156" r:id="rId33" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_155.jpg" xr:uid="{486B1A09-D1FF-4A76-8065-DAF5622FEE85}"/>
+    <hyperlink ref="F157" r:id="rId34" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_156.jpg" xr:uid="{27D8A5BE-EAB4-4EA1-A209-A799E4972A33}"/>
+    <hyperlink ref="F158" r:id="rId35" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_157.jpg" xr:uid="{3DED97D7-548F-43C5-AFEB-0E42878C7F16}"/>
+    <hyperlink ref="F159" r:id="rId36" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_158.jpg" xr:uid="{C40836AF-253B-4968-A180-3D778F4B000D}"/>
+    <hyperlink ref="F160" r:id="rId37" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_159.jpg" xr:uid="{70760C64-1062-467B-B493-B3D18A67C06D}"/>
+    <hyperlink ref="F161" r:id="rId38" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_160.jpg" xr:uid="{1751117D-F718-42AA-8EEF-C314BD4E6EDD}"/>
+    <hyperlink ref="F162" r:id="rId39" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_161.jpg" xr:uid="{C2D46308-E84C-4EB6-A2A7-F0CD5644B86A}"/>
+    <hyperlink ref="F163" r:id="rId40" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_162.jpg" xr:uid="{D9E751C4-57E6-4426-AD5B-E8E35CA711A8}"/>
+    <hyperlink ref="F164" r:id="rId41" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_163.jpg" xr:uid="{1E3090DE-5F14-40A0-B068-FA0410047228}"/>
+    <hyperlink ref="F165" r:id="rId42" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_164.jpg" xr:uid="{000BA945-168D-4514-BA43-5983EFFE571D}"/>
+    <hyperlink ref="F166" r:id="rId43" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_165.jpg" xr:uid="{41C1DC10-A3EB-4671-A787-A8B6D8D6C4E6}"/>
+    <hyperlink ref="F167" r:id="rId44" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_166.jpg" xr:uid="{A0DED850-9723-4A31-BAD8-4CCDD469CE9D}"/>
+    <hyperlink ref="F168" r:id="rId45" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_167.jpg" xr:uid="{BADB420B-5F67-48A7-901E-9D9F0A85E49A}"/>
+    <hyperlink ref="F2" r:id="rId46" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_001.JPG" xr:uid="{D43A0608-3025-4E10-8E2E-5311FC61D4B4}"/>
+    <hyperlink ref="F7" r:id="rId47" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_006.jpeg" xr:uid="{076A97D8-03AD-4176-9564-55FABF74946B}"/>
+    <hyperlink ref="F11" r:id="rId48" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_010.jpeg" xr:uid="{AA7039FA-CD6C-4742-8C77-40090A0B41D6}"/>
+    <hyperlink ref="F13" r:id="rId49" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_012.jpeg" xr:uid="{13F311E4-36BA-4CFD-998B-C1E9EDAEDD6C}"/>
+    <hyperlink ref="F35" r:id="rId50" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_034.jpeg" xr:uid="{BA484B96-6FE5-4E91-A6B9-A3AE8C72FABE}"/>
+    <hyperlink ref="F38" r:id="rId51" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_037.jpeg" xr:uid="{6B26CD61-05BD-4FBE-99EA-69638465E280}"/>
+    <hyperlink ref="F50" r:id="rId52" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_049.jpeg" xr:uid="{28E0AAFD-810A-4D4B-808B-C26BE5C7FDF9}"/>
+    <hyperlink ref="F69" r:id="rId53" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_068.jpeg" xr:uid="{14C00680-EB91-4078-A7EB-7CDD767B6010}"/>
+    <hyperlink ref="F71" r:id="rId54" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_070.jpeg" xr:uid="{C6DF508C-65F2-4339-85EE-0627C6CB9023}"/>
+    <hyperlink ref="F73" r:id="rId55" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_072.jpeg" xr:uid="{D349BC95-A2D9-41A1-85BC-A99C7E9055CE}"/>
+    <hyperlink ref="F75" r:id="rId56" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_074.jpeg" xr:uid="{6A58F0CE-BA52-47BB-A249-7C0BC00EDCCC}"/>
+    <hyperlink ref="F92" r:id="rId57" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_091.jpeg" xr:uid="{B70BF618-8F37-4856-B7C7-2DD4686C8938}"/>
+    <hyperlink ref="F169" r:id="rId58" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg" xr:uid="{72875193-4BB9-4298-B334-D45C032E669B}"/>
+    <hyperlink ref="F170" r:id="rId59" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg" xr:uid="{7CFC5301-A5E3-4A5D-97C6-A4C0EE0406AE}"/>
+    <hyperlink ref="F171" r:id="rId60" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg" xr:uid="{D4992F6F-89C9-4647-94B6-6C8589D74789}"/>
+    <hyperlink ref="F172" r:id="rId61" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg" xr:uid="{3ED0D14C-F5A3-4C07-873B-BDA1D1C0A1D6}"/>
+    <hyperlink ref="F173" r:id="rId62" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_172.jpg" xr:uid="{8DD6AC65-41C0-4879-835C-BBF947A1FED4}"/>
+    <hyperlink ref="F174" r:id="rId63" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_173.jpg" xr:uid="{65D2A0A5-63D9-4E7C-92FA-A797E8CB9E28}"/>
+    <hyperlink ref="F175" r:id="rId64" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_174.jpg" xr:uid="{8A4ADCD1-3C0B-4AFF-8BAF-237C74CC9224}"/>
+    <hyperlink ref="F176" r:id="rId65" display="https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg" xr:uid="{218C2329-C30A-4A9F-81F1-5E084F34D55D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId66"/>

</xml_diff>

<commit_message>
update xlsx and puz_data.js
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/Temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/website/DALeske.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD7D6C45-0187-47FA-A43E-0C18CFF39232}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
   </bookViews>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4443A7F1-90C3-4D7D-8B82-1D6A6D8DE156}">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C156" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169:G176"/>
+    <sheetView tabSelected="1" topLeftCell="C163" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,8 +1784,8 @@
         <v>406</v>
       </c>
       <c r="G2" t="str">
-        <f>CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F2&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "1","Title": "Lighthouse","Pieces": "500","Company": "Re-marks","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_001.JPG"</v>
+        <f>"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F2&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "1","Title": "Lighthouse","Pieces": "500","Company": "Re-marks","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_001.JPG"},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1808,8 +1808,8 @@
         <v>252</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" si="0">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F3&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "2","Title": "Cakes","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_002.jpg"</v>
+        <f t="shared" ref="G3:G66" si="0">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F3&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "2","Title": "Cakes","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_002.jpg"},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "3","Title": "More Ice Cream Please","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_003.jpg"</v>
+        <v>{"PuzzleNum": "3","Title": "More Ice Cream Please","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_003.jpg"},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "4","Title": "Artsy Cats","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_004.jpg"</v>
+        <v>{"PuzzleNum": "4","Title": "Artsy Cats","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_004.jpg"},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "5","Title": "Air Mail","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_005.jpg"</v>
+        <v>{"PuzzleNum": "5","Title": "Air Mail","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_005.jpg"},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_006.jpeg"</v>
+        <v>{"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_006.jpeg"},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "7","Title": "Kitchen Cupboard","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_007.jpg"</v>
+        <v>{"PuzzleNum": "7","Title": "Kitchen Cupboard","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_007.jpg"},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "8","Title": "99 Beautiful Places","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_008.jpg"</v>
+        <v>{"PuzzleNum": "8","Title": "99 Beautiful Places","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_008.jpg"},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "9","Title": "Songbirds","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_009.jpg"</v>
+        <v>{"PuzzleNum": "9","Title": "Songbirds","Pieces": "500","Company": "Mudpuppy","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_009.jpg"},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "10","Title": "Marbles","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_010.jpeg"</v>
+        <v>{"PuzzleNum": "10","Title": "Marbles","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_010.jpeg"},</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "11","Title": "60 American National Parks","Pieces": "500","Company": "True South","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_011.jpg"</v>
+        <v>{"PuzzleNum": "11","Title": "60 American National Parks","Pieces": "500","Company": "True South","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_011.jpg"},</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "12","Title": "Visting the Mansion","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_012.jpeg"</v>
+        <v>{"PuzzleNum": "12","Title": "Visting the Mansion","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_012.jpeg"},</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "13","Title": "Black Beauty Carousel Horse","Pieces": "500","Company": "Colorluxe","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_013.jpg"</v>
+        <v>{"PuzzleNum": "13","Title": "Black Beauty Carousel Horse","Pieces": "500","Company": "Colorluxe","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_013.jpg"},</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "14","Title": "Teddy Bear Workshop","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_014.jpg"</v>
+        <v>{"PuzzleNum": "14","Title": "Teddy Bear Workshop","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_014.jpg"},</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "15","Title": "Doughnuts","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_015.jpg"</v>
+        <v>{"PuzzleNum": "15","Title": "Doughnuts","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_015.jpg"},</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "16","Title": "Pretty Birds","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_016.jpg"</v>
+        <v>{"PuzzleNum": "16","Title": "Pretty Birds","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_016.jpg"},</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "17","Title": "Bicycle","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_017.jpg"</v>
+        <v>{"PuzzleNum": "17","Title": "Bicycle","Pieces": "500","Company": "Re-marks","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_017.jpg"},</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "18","Title": "Spring Flowers","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_018.jpg"</v>
+        <v>{"PuzzleNum": "18","Title": "Spring Flowers","Pieces": "500","Company": "Galison","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_018.jpg"},</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "19","Title": "The Bizarre Workshop","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_019.jpg"</v>
+        <v>{"PuzzleNum": "19","Title": "The Bizarre Workshop","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_019.jpg"},</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "20","Title": "Floral Reflections","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_020.jpg"</v>
+        <v>{"PuzzleNum": "20","Title": "Floral Reflections","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_020.jpg"},</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "21","Title": "Snack Treats","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_021.jpg"</v>
+        <v>{"PuzzleNum": "21","Title": "Snack Treats","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_021.jpg"},</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "22","Title": "Oh Buoy!","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_022.jpg"</v>
+        <v>{"PuzzleNum": "22","Title": "Oh Buoy!","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_022.jpg"},</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "23","Title": "Colorful Yarn","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_023.jpg"</v>
+        <v>{"PuzzleNum": "23","Title": "Colorful Yarn","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_023.jpg"},</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "24","Title": "Butterfly Frenzy","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_024.jpg"</v>
+        <v>{"PuzzleNum": "24","Title": "Butterfly Frenzy","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_024.jpg"},</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "25","Title": "Shelter From the Storm","Pieces": "500","Company": "Bits and Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_025.jpg"</v>
+        <v>{"PuzzleNum": "25","Title": "Shelter From the Storm","Pieces": "500","Company": "Bits and Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_025.jpg"},</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "26","Title": "Prima Ballerina","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_026.jpg"</v>
+        <v>{"PuzzleNum": "26","Title": "Prima Ballerina","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_026.jpg"},</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "27","Title": "A Licenese to Life","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_027.jpg"</v>
+        <v>{"PuzzleNum": "27","Title": "A Licenese to Life","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_027.jpg"},</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "28","Title": "Donuts n' Coffee","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_028.jpg"</v>
+        <v>{"PuzzleNum": "28","Title": "Donuts n' Coffee","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_028.jpg"},</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "29","Title": "Pencil Pushers","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_029.jpg"</v>
+        <v>{"PuzzleNum": "29","Title": "Pencil Pushers","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_029.jpg"},</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "30","Title": "Christmas Creations","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_030.jpg"</v>
+        <v>{"PuzzleNum": "30","Title": "Christmas Creations","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_030.jpg"},</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "31","Title": "Winters Wish","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_031.jpg"</v>
+        <v>{"PuzzleNum": "31","Title": "Winters Wish","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_031.jpg"},</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "32","Title": "Delightful Donuts","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_032.jpg"</v>
+        <v>{"PuzzleNum": "32","Title": "Delightful Donuts","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_032.jpg"},</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "33","Title": "Succulents","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_033.jpg"</v>
+        <v>{"PuzzleNum": "33","Title": "Succulents","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_033.jpg"},</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "34","Title": "Sushi","Pieces": "550","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_034.jpeg"</v>
+        <v>{"PuzzleNum": "34","Title": "Sushi","Pieces": "550","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_034.jpeg"},</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "35","Title": "Bon Appetit","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_035.jpg"</v>
+        <v>{"PuzzleNum": "35","Title": "Bon Appetit","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_035.jpg"},</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "36","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_036.jpg"</v>
+        <v>{"PuzzleNum": "36","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_036.jpg"},</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "37","Title": "Root Beer at the Butterfields","Pieces": "300","Company": "Buffalo","Size": "21.5 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_037.jpeg"</v>
+        <v>{"PuzzleNum": "37","Title": "Root Beer at the Butterfields","Pieces": "300","Company": "Buffalo","Size": "21.5 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_037.jpeg"},</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "38","Title": "Donut Resist","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_038.jpg"</v>
+        <v>{"PuzzleNum": "38","Title": "Donut Resist","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_038.jpg"},</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "39","Title": "Este' MacLeod","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_039.jpg"</v>
+        <v>{"PuzzleNum": "39","Title": "Este' MacLeod","Pieces": "300","Company": "Ceaco","Size": "19 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_039.jpg"},</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "40","Title": "Mickey and Minnie in Paris","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_040.jpg"</v>
+        <v>{"PuzzleNum": "40","Title": "Mickey and Minnie in Paris","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_040.jpg"},</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "41","Title": "Rainbow Buttons","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_041.jpg"</v>
+        <v>{"PuzzleNum": "41","Title": "Rainbow Buttons","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_041.jpg"},</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "42","Title": "Frederick the Literate","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_042.jpg"</v>
+        <v>{"PuzzleNum": "42","Title": "Frederick the Literate","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_042.jpg"},</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "43","Title": "Bobons, Sweets, Dulces","Pieces": "750","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_043.jpg"</v>
+        <v>{"PuzzleNum": "43","Title": "Bobons, Sweets, Dulces","Pieces": "750","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_043.jpg"},</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "44","Title": "Seaside","Pieces": "750","Company": "Ceaco","Size": "24 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_044.jpg"</v>
+        <v>{"PuzzleNum": "44","Title": "Seaside","Pieces": "750","Company": "Ceaco","Size": "24 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_044.jpg"},</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "45","Title": "Beachcombers","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_045.jpg"</v>
+        <v>{"PuzzleNum": "45","Title": "Beachcombers","Pieces": "750","Company": "Buffalo","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_045.jpg"},</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "46","Title": "Rainbow Marbles","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_046.jpg"</v>
+        <v>{"PuzzleNum": "46","Title": "Rainbow Marbles","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_046.jpg"},</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "47","Title": "License Plates","Pieces": "750","Company": "Re-marks","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_047.jpg"</v>
+        <v>{"PuzzleNum": "47","Title": "License Plates","Pieces": "750","Company": "Re-marks","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_047.jpg"},</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "48","Title": "Plumes of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_048.jpg"</v>
+        <v>{"PuzzleNum": "48","Title": "Plumes of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_048.jpg"},</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "49","Title": "Autumn Sail","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_049.jpeg"</v>
+        <v>{"PuzzleNum": "49","Title": "Autumn Sail","Pieces": "300","Company": "Master Pieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_049.jpeg"},</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "50","Title": "Mandala Stones","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_050.jpg"</v>
+        <v>{"PuzzleNum": "50","Title": "Mandala Stones","Pieces": "300","Company": "Buffalo","Size": "18 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_050.jpg"},</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "51","Title": "Grandiose Greece","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_051.jpg"</v>
+        <v>{"PuzzleNum": "51","Title": "Grandiose Greece","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_051.jpg"},</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "52","Title": "Garden Bridge","Pieces": "1000","Company": "Master Pieces","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_052.jpg"</v>
+        <v>{"PuzzleNum": "52","Title": "Garden Bridge","Pieces": "1000","Company": "Master Pieces","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_052.jpg"},</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "53","Title": "Drops of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_053.jpg"</v>
+        <v>{"PuzzleNum": "53","Title": "Drops of Color","Pieces": "300","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_053.jpg"},</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "54","Title": "Rainbow Clownfish","Pieces": "550","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_054.jpg"</v>
+        <v>{"PuzzleNum": "54","Title": "Rainbow Clownfish","Pieces": "550","Company": "Ceaco","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_054.jpg"},</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "55","Title": "Banana Split","Pieces": "1000","Company": "Buffalo","Size": "26.75 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_055.jpg"</v>
+        <v>{"PuzzleNum": "55","Title": "Banana Split","Pieces": "1000","Company": "Buffalo","Size": "26.75 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_055.jpg"},</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "56","Title": "Harry Potter Collage","Pieces": "1000","Company": "New York Puzzle Company","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_056.jpg"</v>
+        <v>{"PuzzleNum": "56","Title": "Harry Potter Collage","Pieces": "1000","Company": "New York Puzzle Company","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_056.jpg"},</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "57","Title": "Happiness Blooms","Pieces": "500","Company": "Lang","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_057.jpg"</v>
+        <v>{"PuzzleNum": "57","Title": "Happiness Blooms","Pieces": "500","Company": "Lang","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_057.jpg"},</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "58","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_058.jpg"</v>
+        <v>{"PuzzleNum": "58","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_058.jpg"},</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "59","Title": "Escape Puzzle","Pieces": "759","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_059.jpg"</v>
+        <v>{"PuzzleNum": "59","Title": "Escape Puzzle","Pieces": "759","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_059.jpg"},</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "60","Title": "Icing on the Cake","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_060.jpg"</v>
+        <v>{"PuzzleNum": "60","Title": "Icing on the Cake","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_060.jpg"},</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "61","Title": "Harvest Festival","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_061.jpg"</v>
+        <v>{"PuzzleNum": "61","Title": "Harvest Festival","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_061.jpg"},</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "62","Title": "Ski Park City","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_062.jpg"</v>
+        <v>{"PuzzleNum": "62","Title": "Ski Park City","Pieces": "500","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_062.jpg"},</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "63","Title": "Three Little Pigs","Pieces": "100","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_063.jpg"</v>
+        <v>{"PuzzleNum": "63","Title": "Three Little Pigs","Pieces": "100","Company": "Dowdle","Size": "20 X 16","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_063.jpg"},</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "64","Title": "Ice Cream Dream","Pieces": "1000","Company": "Chronicle Books","Size": "25 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_064.jpg"</v>
+        <v>{"PuzzleNum": "64","Title": "Ice Cream Dream","Pieces": "1000","Company": "Chronicle Books","Size": "25 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_064.jpg"},</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v>"PuzzleNum": "65","Title": "Marvel","Pieces": "1000","Company": "Aquarius","Size": "20 X 28","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_065.jpg"</v>
+        <v>{"PuzzleNum": "65","Title": "Marvel","Pieces": "1000","Company": "Aquarius","Size": "20 X 28","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_065.jpg"},</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -3344,8 +3344,8 @@
         <v>310</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G130" si="1">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F67&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "66","Title": "Feathered Friends","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_066.jpg"</v>
+        <f t="shared" ref="G67:G130" si="1">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F67&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "66","Title": "Feathered Friends","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_066.jpg"},</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "67","Title": "Board Games","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_067.jpg"</v>
+        <v>{"PuzzleNum": "67","Title": "Board Games","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_067.jpg"},</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "68","Title": "Cookies &amp; Christmas","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_068.jpeg"</v>
+        <v>{"PuzzleNum": "68","Title": "Cookies &amp; Christmas","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_068.jpeg"},</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "69","Title": "Cupcakes","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_069.jpg"</v>
+        <v>{"PuzzleNum": "69","Title": "Cupcakes","Pieces": "350","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_069.jpg"},</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "70","Title": "Ship Portal","Pieces": "100","Company": "Great American Puzzle Factory","Size": "13 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_070.jpeg"</v>
+        <v>{"PuzzleNum": "70","Title": "Ship Portal","Pieces": "100","Company": "Great American Puzzle Factory","Size": "13 round","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_070.jpeg"},</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "71","Title": "Minnesota Nice up North","Pieces": "550","Company": "Puzzles that Rock","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_071.jpg"</v>
+        <v>{"PuzzleNum": "71","Title": "Minnesota Nice up North","Pieces": "550","Company": "Puzzles that Rock","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_071.jpg"},</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "72","Title": "Lake Superior Agates","Pieces": "550","Company": "Erickson Post","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_072.jpeg"</v>
+        <v>{"PuzzleNum": "72","Title": "Lake Superior Agates","Pieces": "550","Company": "Erickson Post","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_072.jpeg"},</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "73","Title": "Vintage Library","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_073.jpg"</v>
+        <v>{"PuzzleNum": "73","Title": "Vintage Library","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_073.jpg"},</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "74","Title": "Butterflies Rock Puddingstone Perch","Pieces": "550","Company": "Puzzle that Rock","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_074.jpeg"</v>
+        <v>{"PuzzleNum": "74","Title": "Butterflies Rock Puddingstone Perch","Pieces": "550","Company": "Puzzle that Rock","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_074.jpeg"},</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "75","Title": "Sea Horsing Around","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_075.jpg"</v>
+        <v>{"PuzzleNum": "75","Title": "Sea Horsing Around","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_075.jpg"},</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "76","Title": "Grandma's Cookies","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_076.jpg"</v>
+        <v>{"PuzzleNum": "76","Title": "Grandma's Cookies","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_076.jpg"},</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "77","Title": "Chocolate Overload","Pieces": "300","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_077.jpg"</v>
+        <v>{"PuzzleNum": "77","Title": "Chocolate Overload","Pieces": "300","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_077.jpg"},</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "78","Title": "Doggie Delight","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_078.jpg"</v>
+        <v>{"PuzzleNum": "78","Title": "Doggie Delight","Pieces": "300","Company": "Ravensburger","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_078.jpg"},</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "79","Title": "Beautiful Horses","Pieces": "200","Company": "Ravensburger","Size": "14.25 X 19.3","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_079.jpg"</v>
+        <v>{"PuzzleNum": "79","Title": "Beautiful Horses","Pieces": "200","Company": "Ravensburger","Size": "14.25 X 19.3","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_079.jpg"},</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "80","Title": "The Fishing Cabin","Pieces": "1000","Company": "Eurographics","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_080.jpg"</v>
+        <v>{"PuzzleNum": "80","Title": "The Fishing Cabin","Pieces": "1000","Company": "Eurographics","Size": "26.75 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_080.jpg"},</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "81","Title": "Peace and Joy","Pieces": "1000","Company": "Go! Games","Size": "19.6 X 29.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_081.jpg"</v>
+        <v>{"PuzzleNum": "81","Title": "Peace and Joy","Pieces": "1000","Company": "Go! Games","Size": "19.6 X 29.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_081.jpg"},</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "82","Title": "Horse Dream","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_082.jpg"</v>
+        <v>{"PuzzleNum": "82","Title": "Horse Dream","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_082.jpg"},</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "83","Title": "WIld Jungle","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_083.jpg"</v>
+        <v>{"PuzzleNum": "83","Title": "WIld Jungle","Pieces": "100","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_083.jpg"},</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3777,7 +3777,7 @@
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "84","Title": "The Solar System","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_084.jpg"</v>
+        <v>{"PuzzleNum": "84","Title": "The Solar System","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_084.jpg"},</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "85","Title": "The Christmas Fair","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_085.jpg"</v>
+        <v>{"PuzzleNum": "85","Title": "The Christmas Fair","Pieces": "200","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_085.jpg"},</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "86","Title": "The Imaginaries","Pieces": "300","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_086.jpg"</v>
+        <v>{"PuzzleNum": "86","Title": "The Imaginaries","Pieces": "300","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_086.jpg"},</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "87","Title": "Sweet Tooth","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_087.jpg"</v>
+        <v>{"PuzzleNum": "87","Title": "Sweet Tooth","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_087.jpg"},</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "88","Title": "Go Fly a Kite","Pieces": "380","Company": "Ravensburger","Size": "26.6 X 10.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_088.jpg"</v>
+        <v>{"PuzzleNum": "88","Title": "Go Fly a Kite","Pieces": "380","Company": "Ravensburger","Size": "26.6 X 10.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_088.jpg"},</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "89","Title": "MN Abbey Road","Pieces": "500","Company": "Maynards","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_089.jpg"</v>
+        <v>{"PuzzleNum": "89","Title": "MN Abbey Road","Pieces": "500","Company": "Maynards","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_089.jpg"},</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "90","Title": "Song for the Season","Pieces": "500","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_090.jpg"</v>
+        <v>{"PuzzleNum": "90","Title": "Song for the Season","Pieces": "500","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_090.jpg"},</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "91","Title": "Father's Day Ties","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_091.jpeg"</v>
+        <v>{"PuzzleNum": "91","Title": "Father's Day Ties","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_091.jpeg"},</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "92","Title": "Welcome to My Garden","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_092.jpg"</v>
+        <v>{"PuzzleNum": "92","Title": "Welcome to My Garden","Pieces": "500","Company": "Cobble Hill","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_092.jpg"},</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "93","Title": "Love, Home, Family, Friends","Pieces": "400","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_093.jpg"</v>
+        <v>{"PuzzleNum": "93","Title": "Love, Home, Family, Friends","Pieces": "400","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_093.jpg"},</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "94","Title": "Autumn Birds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_094.jpg"</v>
+        <v>{"PuzzleNum": "94","Title": "Autumn Birds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_094.jpg"},</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "95","Title": "Drive-thru Route 66","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_095.jpg"</v>
+        <v>{"PuzzleNum": "95","Title": "Drive-thru Route 66","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_095.jpg"},</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "96","Title": "Weekend Escape","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_096.jpg"</v>
+        <v>{"PuzzleNum": "96","Title": "Weekend Escape","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_096.jpg"},</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="G98" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "97","Title": "Underwater Smiles","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_097.jpg"</v>
+        <v>{"PuzzleNum": "97","Title": "Underwater Smiles","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_097.jpg"},</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="G99" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "98","Title": "Minnesota Spirit","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_098.jpg"</v>
+        <v>{"PuzzleNum": "98","Title": "Minnesota Spirit","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_098.jpg"},</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="G100" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "99","Title": "State Plates","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_099.jpg"</v>
+        <v>{"PuzzleNum": "99","Title": "State Plates","Pieces": "400","Company": "Springbok","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_099.jpg"},</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="G101" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "100","Title": "Cabin Rules","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_100.jpg"</v>
+        <v>{"PuzzleNum": "100","Title": "Cabin Rules","Pieces": "1000","Company": "Puzzle Twist","Size": "19.25 X 26.6","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_100.jpg"},</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="G102" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "101","Title": "Boat Parade","Pieces": "1000","Company": "Spilsbury Puzzle Co","Size": "26.75 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_101.jpg"</v>
+        <v>{"PuzzleNum": "101","Title": "Boat Parade","Pieces": "1000","Company": "Spilsbury Puzzle Co","Size": "26.75 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_101.jpg"},</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "102","Title": "A Rainbow in Bloom","Pieces": "70","Company": "Springbok","Size": "7 X 7 (Qty 6)","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_102.jpg"</v>
+        <v>{"PuzzleNum": "102","Title": "A Rainbow in Bloom","Pieces": "70","Company": "Springbok","Size": "7 X 7 (Qty 6)","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_102.jpg"},</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="G104" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "103","Title": "Candy Galore","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_103.jpg"</v>
+        <v>{"PuzzleNum": "103","Title": "Candy Galore","Pieces": "1000","Company": "Springbok","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_103.jpg"},</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "104","Title": "Ugly Christmas Sweaters","Pieces": "1000","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_104.jpg"</v>
+        <v>{"PuzzleNum": "104","Title": "Ugly Christmas Sweaters","Pieces": "1000","Company": "Cobble Hill","Size": "26.6 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_104.jpg"},</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -4281,7 +4281,7 @@
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "105","Title": "The Artist's Desk","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_105.jpg"</v>
+        <v>{"PuzzleNum": "105","Title": "The Artist's Desk","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_105.jpg"},</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="G107" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "106","Title": "Disney Pixar Movies","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_106.jpg"</v>
+        <v>{"PuzzleNum": "106","Title": "Disney Pixar Movies","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_106.jpg"},</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="G108" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "107","Title": "Scorceror's Apprentice","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_107.jpg"</v>
+        <v>{"PuzzleNum": "107","Title": "Scorceror's Apprentice","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_107.jpg"},</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="G109" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "108","Title": "Disney Chefs","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_108.jpg"</v>
+        <v>{"PuzzleNum": "108","Title": "Disney Chefs","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_108.jpg"},</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="G110" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_109.jpg"</v>
+        <v>{"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_109.jpg"},</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="G111" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "110","Title": "Sitting Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_110.jpg"</v>
+        <v>{"PuzzleNum": "110","Title": "Sitting Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_110.jpg"},</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="G112" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "111","Title": "Danicing Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_111.jpg"</v>
+        <v>{"PuzzleNum": "111","Title": "Danicing Mickey &amp; Minnie","Pieces": "300","Company": "Ceaco","Size": "11 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_111.jpg"},</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="G113" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_112.jpg"</v>
+        <v>{"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_112.jpg"},</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="G114" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_113.jpg"</v>
+        <v>{"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_113.jpg"},</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="G115" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_114.jpg"</v>
+        <v>{"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_114.jpg"},</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="G116" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_115.jpg"</v>
+        <v>{"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_115.jpg"},</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="G117" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_116.jpg"</v>
+        <v>{"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_116.jpg"},</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="G118" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_117.jpg"</v>
+        <v>{"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_117.jpg"},</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="G119" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_118.jpg"</v>
+        <v>{"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_118.jpg"},</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4614,7 +4614,7 @@
       </c>
       <c r="G120" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "119","Title": "Unknown","Pieces": "1000","Company": "unknown","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_119.jpg"</v>
+        <v>{"PuzzleNum": "119","Title": "Unknown","Pieces": "1000","Company": "unknown","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_119.jpg"},</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="G121" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "120","Title": "Family Vacation","Pieces": "2000","Company": "Buffalo","Size": "38.5 X 26.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_120.jpg"</v>
+        <v>{"PuzzleNum": "120","Title": "Family Vacation","Pieces": "2000","Company": "Buffalo","Size": "38.5 X 26.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_120.jpg"},</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="G122" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "121","Title": "Ideal Bookshelf","Pieces": "1000","Company": "Galison","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_121.jpg"</v>
+        <v>{"PuzzleNum": "121","Title": "Ideal Bookshelf","Pieces": "1000","Company": "Galison","Size": "27 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_121.jpg"},</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="G123" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "122","Title": "Singbird Serenade","Pieces": "500","Company": "Puzzle Twist","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_122.jpg"</v>
+        <v>{"PuzzleNum": "122","Title": "Singbird Serenade","Pieces": "500","Company": "Puzzle Twist","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_122.jpg"},</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="G124" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "123","Title": "Underwater Seascape","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_123.jpg"</v>
+        <v>{"PuzzleNum": "123","Title": "Underwater Seascape","Pieces": "500","Company": "Springbok","Size": "23.5 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_123.jpg"},</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="G125" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "124","Title": "The Flintstones","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_124.jpg"</v>
+        <v>{"PuzzleNum": "124","Title": "The Flintstones","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_124.jpg"},</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -4758,7 +4758,7 @@
       </c>
       <c r="G126" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "125","Title": "Scooby-Doo!","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_125.jpg"</v>
+        <v>{"PuzzleNum": "125","Title": "Scooby-Doo!","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_125.jpg"},</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="G127" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "126","Title": "The Jetsons","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_126.jpg"</v>
+        <v>{"PuzzleNum": "126","Title": "The Jetsons","Pieces": "500","Company": "MasterPieces","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_126.jpg"},</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -4806,7 +4806,7 @@
       </c>
       <c r="G128" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "127","Title": "Morning Magic","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_127.jpg"</v>
+        <v>{"PuzzleNum": "127","Title": "Morning Magic","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_127.jpg"},</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4830,7 +4830,7 @@
       </c>
       <c r="G129" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "128","Title": "Circle of Colors: Animals","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_128.jpg"</v>
+        <v>{"PuzzleNum": "128","Title": "Circle of Colors: Animals","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_128.jpg"},</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="G130" t="str">
         <f t="shared" si="1"/>
-        <v>"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_129.jpg"</v>
+        <v>{"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_129.jpg"},</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -4877,8 +4877,8 @@
         <v>368</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" ref="G131:G176" si="2">CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F131&amp;CHAR(34)</f>
-        <v>"PuzzleNum": "130","Title": "Animal Yoga","Pieces": "500","Company": "unknown","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_130.jpg"</v>
+        <f t="shared" ref="G131:G176" si="2">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E131&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F131&amp;CHAR(34)&amp;"},"</f>
+        <v>{"PuzzleNum": "130","Title": "Animal Yoga","Pieces": "500","Company": "unknown","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_130.jpg"},</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="G132" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "131","Title": "Christmas Singbirds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_131.jpg"</v>
+        <v>{"PuzzleNum": "131","Title": "Christmas Singbirds","Pieces": "500","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_131.jpg"},</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -4926,7 +4926,7 @@
       </c>
       <c r="G133" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "132","Title": "Typefaces","Pieces": "500","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_132.jpg"</v>
+        <v>{"PuzzleNum": "132","Title": "Typefaces","Pieces": "500","Company": "Ravensburger","Size": "19.3 X 14.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_132.jpg"},</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="G134" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "133","Title": "Tree of Life","Pieces": "275","Company": "Cobble Hill","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_133.jpg"</v>
+        <v>{"PuzzleNum": "133","Title": "Tree of Life","Pieces": "275","Company": "Cobble Hill","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_133.jpg"},</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -4974,7 +4974,7 @@
       </c>
       <c r="G135" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "134","Title": "MinneSNOWta","Pieces": "500","Company": "PuzzleTwist","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_134.jpg"</v>
+        <v>{"PuzzleNum": "134","Title": "MinneSNOWta","Pieces": "500","Company": "PuzzleTwist","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_134.jpg"},</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="G136" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "135","Title": "Up","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_135.jpg"</v>
+        <v>{"PuzzleNum": "135","Title": "Up","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_135.jpg"},</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -5022,7 +5022,7 @@
       </c>
       <c r="G137" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "136","Title": "San Diego Zoo","Pieces": "500","Company": "San Diego Zoo Wildlife Alliance","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_136.jpg"</v>
+        <v>{"PuzzleNum": "136","Title": "San Diego Zoo","Pieces": "500","Company": "San Diego Zoo Wildlife Alliance","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_136.jpg"},</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -5046,7 +5046,7 @@
       </c>
       <c r="G138" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "137","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_137.jpg"</v>
+        <v>{"PuzzleNum": "137","Title": "Peanuts","Pieces": "500","Company": "Aquarius","Size": "14 X 19","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_137.jpg"},</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -5070,7 +5070,7 @@
       </c>
       <c r="G139" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "138","Title": "Winnie the Pooh","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_138.jpg"</v>
+        <v>{"PuzzleNum": "138","Title": "Winnie the Pooh","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_138.jpg"},</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="G140" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "139","Title": "Scooby Doo Haunted Game","Pieces": "200","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_139.jpg"</v>
+        <v>{"PuzzleNum": "139","Title": "Scooby Doo Haunted Game","Pieces": "200","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_139.jpg"},</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="G141" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "140","Title": "Toy Story","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_140.jpg"</v>
+        <v>{"PuzzleNum": "140","Title": "Toy Story","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_140.jpg"},</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -5139,7 +5139,7 @@
       </c>
       <c r="G142" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "141","Title": "Pups in Cups","Pieces": "500 total","Company": "Rose Art","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_141.jpg"</v>
+        <v>{"PuzzleNum": "141","Title": "Pups in Cups","Pieces": "500 total","Company": "Rose Art","Size": "","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_141.jpg"},</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -5163,7 +5163,7 @@
       </c>
       <c r="G143" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "142","Title": "You Betcha!","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_142.jpg"</v>
+        <v>{"PuzzleNum": "142","Title": "You Betcha!","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_142.jpg"},</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="G144" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "143","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_143.jpg"</v>
+        <v>{"PuzzleNum": "143","Title": "Gnome Sweet Gnome","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_143.jpg"},</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -5211,7 +5211,7 @@
       </c>
       <c r="G145" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "144","Title": "Goofy","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_144.jpg"</v>
+        <v>{"PuzzleNum": "144","Title": "Goofy","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_144.jpg"},</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="G146" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "145","Title": "Barbie Around the World","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_145.jpg"</v>
+        <v>{"PuzzleNum": "145","Title": "Barbie Around the World","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_145.jpg"},</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G147" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "146","Title": "Pooh to the Rescue","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_146.jpg"</v>
+        <v>{"PuzzleNum": "146","Title": "Pooh to the Rescue","Pieces": "100","Company": "Ravensburger","Size": "19 X 14","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_146.jpg"},</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -5283,7 +5283,7 @@
       </c>
       <c r="G148" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_147.jpg"</v>
+        <v>{"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_147.jpg"},</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -5307,7 +5307,7 @@
       </c>
       <c r="G149" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "148","Title": "Gnomes Get Baking","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_148.jpg"</v>
+        <v>{"PuzzleNum": "148","Title": "Gnomes Get Baking","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_148.jpg"},</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -5331,7 +5331,7 @@
       </c>
       <c r="G150" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "149","Title": "Mickey and Friends","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_149.jpg"</v>
+        <v>{"PuzzleNum": "149","Title": "Mickey and Friends","Pieces": "300","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_149.jpg"},</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="G151" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "150","Title": "Coming Home","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_150.jpg"</v>
+        <v>{"PuzzleNum": "150","Title": "Coming Home","Pieces": "750","Company": "Ceaco","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_150.jpg"},</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -5379,7 +5379,7 @@
       </c>
       <c r="G152" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "151","Title": "Sky Roads","Pieces": "1000","Company": "Buffalo","Size": "26.76 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_151.jpg"</v>
+        <v>{"PuzzleNum": "151","Title": "Sky Roads","Pieces": "1000","Company": "Buffalo","Size": "26.76 X 19.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_151.jpg"},</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -5403,7 +5403,7 @@
       </c>
       <c r="G153" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "152","Title": "Front Porch Flag","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_152.jpg"</v>
+        <v>{"PuzzleNum": "152","Title": "Front Porch Flag","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_152.jpg"},</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -5427,7 +5427,7 @@
       </c>
       <c r="G154" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "153","Title": "Springtime Cookies","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_153.jpg"</v>
+        <v>{"PuzzleNum": "153","Title": "Springtime Cookies","Pieces": "500","Company": "Springbok","Size": "18 X 23.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_153.jpg"},</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -5451,7 +5451,7 @@
       </c>
       <c r="G155" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "154","Title": "Tom + Jerry Hall of Fame","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_154.jpg"</v>
+        <v>{"PuzzleNum": "154","Title": "Tom + Jerry Hall of Fame","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_154.jpg"},</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -5475,7 +5475,7 @@
       </c>
       <c r="G156" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "155","Title": "Fruits + Vegetables","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_155.jpg"</v>
+        <v>{"PuzzleNum": "155","Title": "Fruits + Vegetables","Pieces": "500","Company": "Ravensburger","Size": "20.47 diameter","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_155.jpg"},</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -5499,7 +5499,7 @@
       </c>
       <c r="G157" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "156","Title": "Bedtime Stories","Pieces": "1000","Company": "Re-marks","Size": "19.25 X 26.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_156.jpg"</v>
+        <v>{"PuzzleNum": "156","Title": "Bedtime Stories","Pieces": "1000","Company": "Re-marks","Size": "19.25 X 26.75","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_156.jpg"},</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="G158" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "157","Title": "Candy Chrome","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_157.jpg"</v>
+        <v>{"PuzzleNum": "157","Title": "Candy Chrome","Pieces": "500","Company": "Buffalo","Size": "21.25 X 15","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_157.jpg"},</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="G159" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "158","Title": "Fireworks Finale","Pieces": "750","Company": "MasterPieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_158.jpg"</v>
+        <v>{"PuzzleNum": "158","Title": "Fireworks Finale","Pieces": "750","Company": "MasterPieces","Size": "24 X 18","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_158.jpg"},</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -5571,7 +5571,7 @@
       </c>
       <c r="G160" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "159","Title": "Horseplay","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_159.jpg"</v>
+        <v>{"PuzzleNum": "159","Title": "Horseplay","Pieces": "1000","Company": "PuzzleTwist","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_159.jpg"},</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="G161" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "160","Title": "Nordic Love","Pieces": "1000","Company": "PuzzleTwist","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_160.jpg"</v>
+        <v>{"PuzzleNum": "160","Title": "Nordic Love","Pieces": "1000","Company": "PuzzleTwist","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_160.jpg"},</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5619,7 +5619,7 @@
       </c>
       <c r="G162" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "161","Title": "Hitting the Road","Pieces": "500","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_161.jpg"</v>
+        <v>{"PuzzleNum": "161","Title": "Hitting the Road","Pieces": "500","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_161.jpg"},</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -5643,7 +5643,7 @@
       </c>
       <c r="G163" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "162","Title": "VW Gone Places","Pieces": "1000","Company": "Eurographics","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_162.jpg"</v>
+        <v>{"PuzzleNum": "162","Title": "VW Gone Places","Pieces": "1000","Company": "Eurographics","Size": "19.25 X 26.63","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_162.jpg"},</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5667,7 +5667,7 @@
       </c>
       <c r="G164" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "163","Title": "Love at Home","Pieces": "500","Company": "Colorly Love","Size": "16 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_163.jpg"</v>
+        <v>{"PuzzleNum": "163","Title": "Love at Home","Pieces": "500","Company": "Colorly Love","Size": "16 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_163.jpg"},</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5691,7 +5691,7 @@
       </c>
       <c r="G165" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "164","Title": "Childhood Stories","Pieces": "400","Company": "Springbok","Size": "20.5 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_164.jpg"</v>
+        <v>{"PuzzleNum": "164","Title": "Childhood Stories","Pieces": "400","Company": "Springbok","Size": "20.5 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_164.jpg"},</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5715,7 +5715,7 @@
       </c>
       <c r="G166" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "165","Title": "Winter Welcome","Pieces": "1000","Company": "Vermont Christmas Company","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_165.jpg"</v>
+        <v>{"PuzzleNum": "165","Title": "Winter Welcome","Pieces": "1000","Company": "Vermont Christmas Company","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_165.jpg"},</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="G167" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "166","Title": "Christmas Barn Snowman","Pieces": "500","Company": "Bits and Pieces","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_166.jpg"</v>
+        <v>{"PuzzleNum": "166","Title": "Christmas Barn Snowman","Pieces": "500","Company": "Bits and Pieces","Size": "18 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_166.jpg"},</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="G168" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "167","Title": "Farmer's Market Trucks","Pieces": "1000","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_167.jpg"</v>
+        <v>{"PuzzleNum": "167","Title": "Farmer's Market Trucks","Pieces": "1000","Company": "Cobble Hill","Size": "26.63 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_167.jpg"},</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G169" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "168","Title": "Sun and Sea","Pieces": "500","Company": "Ravensburger","Size": "27.5 X 19.67","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg"</v>
+        <v>{"PuzzleNum": "168","Title": "Sun and Sea","Pieces": "500","Company": "Ravensburger","Size": "27.5 X 19.67","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg"},</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg"</v>
+        <v>{"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg"},</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5835,7 +5835,7 @@
       </c>
       <c r="G171" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg"</v>
+        <v>{"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg"},</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5859,7 +5859,7 @@
       </c>
       <c r="G172" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "171","Title": "Jellies &amp; Jams","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg"</v>
+        <v>{"PuzzleNum": "171","Title": "Jellies &amp; Jams","Pieces": "500","Company": "Springbok","Size": "20 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg"},</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="G173" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "172","Title": "Backyard BBQ","Pieces": "1000","Company": "White Mountain","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_172.jpg"</v>
+        <v>{"PuzzleNum": "172","Title": "Backyard BBQ","Pieces": "1000","Company": "White Mountain","Size": "30 X 24","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_172.jpg"},</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G174" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "173","Title": "Blossoms and Kittens Quilt","Pieces": "1000","Company": "Cobble Hill","Size": "26.625 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_173.jpg"</v>
+        <v>{"PuzzleNum": "173","Title": "Blossoms and Kittens Quilt","Pieces": "1000","Company": "Cobble Hill","Size": "26.625 X 19.25","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_173.jpg"},</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="G175" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "174","Title": "Honey and Tea","Pieces": "1000","Company": "Sunsout","Size": "35 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_174.jpg"</v>
+        <v>{"PuzzleNum": "174","Title": "Honey and Tea","Pieces": "1000","Company": "Sunsout","Size": "35 X 27","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_174.jpg"},</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5955,7 +5955,7 @@
       </c>
       <c r="G176" t="str">
         <f t="shared" si="2"/>
-        <v>"PuzzleNum": "175","Title": "Christmas Carolers","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg"</v>
+        <v>{"PuzzleNum": "175","Title": "Christmas Carolers","Pieces": "1000","Company": "Galison","Size": "27 X 20","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg"},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct jpg to jpeg
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/website/DALeske.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD7D6C45-0187-47FA-A43E-0C18CFF39232}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC56C888-2B95-4651-9CCF-61DC0E2D1EF9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
   </bookViews>
@@ -1345,12 +1345,6 @@
     <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_168.jpg</t>
   </si>
   <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg</t>
-  </si>
-  <si>
     <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_171.jpg</t>
   </si>
   <si>
@@ -1364,6 +1358,12 @@
   </si>
   <si>
     <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_175.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1729,7 +1729,7 @@
   <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C163" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G176"/>
+      <selection activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5807,11 +5807,11 @@
         <v>148</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="G170" t="str">
         <f t="shared" si="2"/>
-        <v>{"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpg"},</v>
+        <v>{"PuzzleNum": "169","Title": "O Christmas Treats","Pieces": "500","Company": "Springbok","Size": "26.75 X 20.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_169.jpeg"},</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5831,11 +5831,11 @@
         <v>429</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="G171" t="str">
         <f t="shared" si="2"/>
-        <v>{"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpg"},</v>
+        <v>{"PuzzleNum": "170","Title": "Stylin Snowman","Pieces": "1000","Company": "Current","Size": "19 X 30.5","URL": "https://github.com/DALeske/puzzle/blob/main/static/images/Puzzle_170.jpeg"},</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5855,7 +5855,7 @@
         <v>10</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G172" t="str">
         <f t="shared" si="2"/>
@@ -5879,7 +5879,7 @@
         <v>138</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G173" t="str">
         <f t="shared" si="2"/>
@@ -5903,7 +5903,7 @@
         <v>431</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G174" t="str">
         <f t="shared" si="2"/>
@@ -5927,7 +5927,7 @@
         <v>433</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G175" t="str">
         <f t="shared" si="2"/>
@@ -5951,7 +5951,7 @@
         <v>79</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G176" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
correct puz 6 image link
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/website/DALeske.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{515EA6C1-660E-4D46-95F9-D4F47782B5D6}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73EC258C-554E-473E-9B68-2ABC3BC16653}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
   </bookViews>
@@ -856,9 +856,6 @@
     <t>static/images/Puzzle_005.jpg</t>
   </si>
   <si>
-    <t>static/images/Puzzle_006.jpeg</t>
-  </si>
-  <si>
     <t>static/images/Puzzle_007.jpg</t>
   </si>
   <si>
@@ -1367,6 +1364,9 @@
   </si>
   <si>
     <t>A License to Life</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_006.jpg</t>
   </si>
 </sst>
 </file>
@@ -1732,9 +1732,9 @@
   <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H176"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,14 +1915,14 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>272</v>
+        <v>442</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>{"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "static/images/Puzzle_006.jpeg","Missing":"0"},</v>
+        <v>{"PuzzleNum": "6","Title": "Alpaca Lunch","Pieces": "500","Company": "Ravensburger","Size": "19.5 X 14.25","URL": "static/images/Puzzle_006.jpg","Missing":"0"},</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1966,7 +1966,7 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1990,7 +1990,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -2014,7 +2014,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="str">
@@ -2039,7 +2039,7 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -2063,7 +2063,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="str">
@@ -2088,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -2112,7 +2112,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -2136,7 +2136,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -2160,7 +2160,7 @@
         <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2184,7 +2184,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2235,7 +2235,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2259,7 +2259,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -2283,7 +2283,7 @@
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -2307,7 +2307,7 @@
         <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -2331,7 +2331,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -2355,7 +2355,7 @@
         <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -2379,7 +2379,7 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -2403,7 +2403,7 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -2415,7 +2415,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C28">
         <v>500</v>
@@ -2427,7 +2427,7 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -2451,7 +2451,7 @@
         <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -2502,7 +2502,7 @@
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -2526,7 +2526,7 @@
         <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -2550,7 +2550,7 @@
         <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -2574,7 +2574,7 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -2598,7 +2598,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" t="str">
@@ -2623,7 +2623,7 @@
         <v>58</v>
       </c>
       <c r="F36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -2647,7 +2647,7 @@
         <v>58</v>
       </c>
       <c r="F37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -2671,7 +2671,7 @@
         <v>61</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="str">
@@ -2696,7 +2696,7 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -2720,7 +2720,7 @@
         <v>58</v>
       </c>
       <c r="F40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -2744,7 +2744,7 @@
         <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -2768,7 +2768,7 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -2792,7 +2792,7 @@
         <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -2816,7 +2816,7 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -2840,7 +2840,7 @@
         <v>70</v>
       </c>
       <c r="F45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -2864,7 +2864,7 @@
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -2888,7 +2888,7 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -2912,7 +2912,7 @@
         <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -2936,7 +2936,7 @@
         <v>34</v>
       </c>
       <c r="F49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -2960,7 +2960,7 @@
         <v>7</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="str">
@@ -2985,7 +2985,7 @@
         <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -3009,7 +3009,7 @@
         <v>78</v>
       </c>
       <c r="F52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -3033,7 +3033,7 @@
         <v>80</v>
       </c>
       <c r="F53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -3057,7 +3057,7 @@
         <v>34</v>
       </c>
       <c r="F54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -3081,7 +3081,7 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -3105,7 +3105,7 @@
         <v>84</v>
       </c>
       <c r="F56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -3129,7 +3129,7 @@
         <v>80</v>
       </c>
       <c r="F57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -3153,7 +3153,7 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -3177,7 +3177,7 @@
         <v>91</v>
       </c>
       <c r="F59" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -3201,7 +3201,7 @@
         <v>78</v>
       </c>
       <c r="F60" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -3225,7 +3225,7 @@
         <v>94</v>
       </c>
       <c r="F61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -3249,7 +3249,7 @@
         <v>16</v>
       </c>
       <c r="F62" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -3273,7 +3273,7 @@
         <v>16</v>
       </c>
       <c r="F63" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -3297,7 +3297,7 @@
         <v>16</v>
       </c>
       <c r="F64" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -3321,7 +3321,7 @@
         <v>101</v>
       </c>
       <c r="F65" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -3345,7 +3345,7 @@
         <v>103</v>
       </c>
       <c r="F66" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
@@ -3369,7 +3369,7 @@
         <v>94</v>
       </c>
       <c r="F67" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H130" si="1">"{"&amp;CHAR(34)&amp;"PuzzleNum"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;A67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Title"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;B67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Pieces"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Company"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;D67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Size"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;E67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"URL"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;F67&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;"Missing"&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;G67&amp;CHAR(34)&amp;"},"</f>
@@ -3393,7 +3393,7 @@
         <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
@@ -3417,7 +3417,7 @@
         <v>10</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" t="str">
@@ -3442,7 +3442,7 @@
         <v>94</v>
       </c>
       <c r="F70" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
@@ -3466,7 +3466,7 @@
         <v>110</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" t="str">
@@ -3491,7 +3491,7 @@
         <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
@@ -3515,7 +3515,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" t="str">
@@ -3540,7 +3540,7 @@
         <v>78</v>
       </c>
       <c r="F74" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
@@ -3564,7 +3564,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="str">
@@ -3589,7 +3589,7 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
@@ -3613,7 +3613,7 @@
         <v>120</v>
       </c>
       <c r="F77" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
@@ -3637,7 +3637,7 @@
         <v>78</v>
       </c>
       <c r="F78" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
@@ -3661,7 +3661,7 @@
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
@@ -3685,7 +3685,7 @@
         <v>124</v>
       </c>
       <c r="F80" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
@@ -3709,7 +3709,7 @@
         <v>80</v>
       </c>
       <c r="F81" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
@@ -3733,7 +3733,7 @@
         <v>129</v>
       </c>
       <c r="F82" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
@@ -3757,7 +3757,7 @@
         <v>131</v>
       </c>
       <c r="F83" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
@@ -3781,7 +3781,7 @@
         <v>131</v>
       </c>
       <c r="F84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
@@ -3805,7 +3805,7 @@
         <v>131</v>
       </c>
       <c r="F85" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
@@ -3829,7 +3829,7 @@
         <v>131</v>
       </c>
       <c r="F86" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
@@ -3853,7 +3853,7 @@
         <v>131</v>
       </c>
       <c r="F87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
@@ -3877,7 +3877,7 @@
         <v>137</v>
       </c>
       <c r="F88" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
@@ -3901,7 +3901,7 @@
         <v>139</v>
       </c>
       <c r="F89" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
@@ -3925,7 +3925,7 @@
         <v>26</v>
       </c>
       <c r="F90" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
@@ -3949,7 +3949,7 @@
         <v>143</v>
       </c>
       <c r="F91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
@@ -3973,7 +3973,7 @@
         <v>7</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" t="str">
@@ -3998,7 +3998,7 @@
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
@@ -4022,7 +4022,7 @@
         <v>147</v>
       </c>
       <c r="F94" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
@@ -4046,7 +4046,7 @@
         <v>78</v>
       </c>
       <c r="F95" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
@@ -4070,7 +4070,7 @@
         <v>78</v>
       </c>
       <c r="F96" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         <v>78</v>
       </c>
       <c r="F97" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
@@ -4121,7 +4121,7 @@
         <v>78</v>
       </c>
       <c r="F98" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
@@ -4145,7 +4145,7 @@
         <v>154</v>
       </c>
       <c r="F99" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
@@ -4169,7 +4169,7 @@
         <v>120</v>
       </c>
       <c r="F100" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
@@ -4193,7 +4193,7 @@
         <v>154</v>
       </c>
       <c r="F101" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
@@ -4217,7 +4217,7 @@
         <v>159</v>
       </c>
       <c r="F102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
@@ -4241,7 +4241,7 @@
         <v>161</v>
       </c>
       <c r="F103" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
@@ -4265,7 +4265,7 @@
         <v>137</v>
       </c>
       <c r="F104" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G104">
         <v>2</v>
@@ -4292,7 +4292,7 @@
         <v>143</v>
       </c>
       <c r="F105" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
@@ -4316,7 +4316,7 @@
         <v>78</v>
       </c>
       <c r="F106" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
@@ -4340,7 +4340,7 @@
         <v>78</v>
       </c>
       <c r="F107" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
@@ -4364,7 +4364,7 @@
         <v>167</v>
       </c>
       <c r="F108" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
@@ -4388,7 +4388,7 @@
         <v>7</v>
       </c>
       <c r="F109" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
@@ -4412,7 +4412,7 @@
         <v>167</v>
       </c>
       <c r="F110" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
@@ -4436,7 +4436,7 @@
         <v>171</v>
       </c>
       <c r="F111" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
@@ -4460,7 +4460,7 @@
         <v>171</v>
       </c>
       <c r="F112" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
@@ -4484,7 +4484,7 @@
         <v>175</v>
       </c>
       <c r="F113" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
@@ -4508,7 +4508,7 @@
         <v>91</v>
       </c>
       <c r="F114" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
@@ -4532,7 +4532,7 @@
         <v>178</v>
       </c>
       <c r="F115" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
@@ -4556,7 +4556,7 @@
         <v>91</v>
       </c>
       <c r="F116" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
@@ -4580,7 +4580,7 @@
         <v>91</v>
       </c>
       <c r="F117" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
@@ -4604,7 +4604,7 @@
         <v>175</v>
       </c>
       <c r="F118" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
@@ -4628,7 +4628,7 @@
         <v>91</v>
       </c>
       <c r="F119" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
@@ -4649,7 +4649,7 @@
         <v>184</v>
       </c>
       <c r="F120" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
@@ -4673,7 +4673,7 @@
         <v>186</v>
       </c>
       <c r="F121" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
@@ -4697,7 +4697,7 @@
         <v>120</v>
       </c>
       <c r="F122" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
@@ -4721,7 +4721,7 @@
         <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
@@ -4745,7 +4745,7 @@
         <v>41</v>
       </c>
       <c r="F124" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
@@ -4769,7 +4769,7 @@
         <v>192</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" t="str">
@@ -4794,7 +4794,7 @@
         <v>192</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" t="str">
@@ -4819,7 +4819,7 @@
         <v>192</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="str">
@@ -4844,7 +4844,7 @@
         <v>34</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" t="str">
@@ -4869,7 +4869,7 @@
         <v>198</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" t="str">
@@ -4894,7 +4894,7 @@
         <v>78</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" t="str">
@@ -4919,7 +4919,7 @@
         <v>7</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G131" s="1"/>
       <c r="H131" t="str">
@@ -4944,7 +4944,7 @@
         <v>78</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" t="str">
@@ -4969,7 +4969,7 @@
         <v>131</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G133" s="1"/>
       <c r="H133" t="str">
@@ -4994,7 +4994,7 @@
         <v>26</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" t="str">
@@ -5019,7 +5019,7 @@
         <v>26</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" t="str">
@@ -5044,7 +5044,7 @@
         <v>7</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" t="str">
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" t="str">
@@ -5094,7 +5094,7 @@
         <v>192</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" t="str">
@@ -5119,7 +5119,7 @@
         <v>78</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" t="str">
@@ -5144,7 +5144,7 @@
         <v>91</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G140" s="1"/>
       <c r="H140" t="str">
@@ -5169,7 +5169,7 @@
         <v>91</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" t="str">
@@ -5191,7 +5191,7 @@
         <v>214</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G142" s="1"/>
       <c r="H142" t="str">
@@ -5216,7 +5216,7 @@
         <v>216</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" t="str">
@@ -5241,7 +5241,7 @@
         <v>7</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" t="str">
@@ -5266,7 +5266,7 @@
         <v>78</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G145" s="1"/>
       <c r="H145" t="str">
@@ -5291,7 +5291,7 @@
         <v>78</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G146" s="1"/>
       <c r="H146" t="str">
@@ -5316,7 +5316,7 @@
         <v>91</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G147" s="1"/>
       <c r="H147" t="str">
@@ -5341,7 +5341,7 @@
         <v>222</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" t="str">
@@ -5366,7 +5366,7 @@
         <v>7</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G149" s="1"/>
       <c r="H149" t="str">
@@ -5391,7 +5391,7 @@
         <v>7</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" t="str">
@@ -5416,7 +5416,7 @@
         <v>7</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G151" s="1"/>
       <c r="H151" t="str">
@@ -5441,7 +5441,7 @@
         <v>227</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G152" s="1"/>
       <c r="H152" t="str">
@@ -5466,7 +5466,7 @@
         <v>34</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G153" s="1"/>
       <c r="H153" t="str">
@@ -5491,7 +5491,7 @@
         <v>94</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G154" s="1"/>
       <c r="H154" t="str">
@@ -5516,7 +5516,7 @@
         <v>78</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" t="str">
@@ -5541,7 +5541,7 @@
         <v>198</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G156" s="1"/>
       <c r="H156" t="str">
@@ -5566,7 +5566,7 @@
         <v>233</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G157" s="1"/>
       <c r="H157" t="str">
@@ -5591,7 +5591,7 @@
         <v>34</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G158" s="1"/>
       <c r="H158" t="str">
@@ -5616,7 +5616,7 @@
         <v>7</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G159" s="1"/>
       <c r="H159" t="str">
@@ -5641,7 +5641,7 @@
         <v>216</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G160" s="1"/>
       <c r="H160" t="str">
@@ -5666,7 +5666,7 @@
         <v>238</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G161" s="1"/>
       <c r="H161" t="str">
@@ -5691,7 +5691,7 @@
         <v>216</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G162" s="1"/>
       <c r="H162" t="str">
@@ -5716,7 +5716,7 @@
         <v>238</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G163" s="1"/>
       <c r="H163" t="str">
@@ -5741,7 +5741,7 @@
         <v>243</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G164" s="1"/>
       <c r="H164" t="str">
@@ -5766,7 +5766,7 @@
         <v>245</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G165" s="1"/>
       <c r="H165" t="str">
@@ -5791,7 +5791,7 @@
         <v>216</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G166" s="1"/>
       <c r="H166" t="str">
@@ -5816,7 +5816,7 @@
         <v>26</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G167" s="1"/>
       <c r="H167" t="str">
@@ -5841,7 +5841,7 @@
         <v>216</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G168" s="1"/>
       <c r="H168" t="str">
@@ -5866,7 +5866,7 @@
         <v>259</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G169" s="1"/>
       <c r="H169" t="str">
@@ -5891,7 +5891,7 @@
         <v>147</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G170" s="1"/>
       <c r="H170" t="str">
@@ -5916,7 +5916,7 @@
         <v>261</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G171" s="1"/>
       <c r="H171" t="str">
@@ -5941,7 +5941,7 @@
         <v>10</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G172" s="1"/>
       <c r="H172" t="str">
@@ -5966,7 +5966,7 @@
         <v>137</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G173" s="1"/>
       <c r="H173" t="str">
@@ -5991,7 +5991,7 @@
         <v>263</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G174" s="1"/>
       <c r="H174" t="str">
@@ -6016,7 +6016,7 @@
         <v>265</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G175" s="1"/>
       <c r="H175" t="str">
@@ -6041,7 +6041,7 @@
         <v>78</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" t="str">

</xml_diff>

<commit_message>
add unknown and correct extensions for image links
</commit_message>
<xml_diff>
--- a/Leske_puzzle_list.xlsx
+++ b/Leske_puzzle_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fef6c3db25312ee/Desktop/website/DALeske.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73EC258C-554E-473E-9B68-2ABC3BC16653}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{3A17EE45-64CA-461F-ADA6-B60A11F4E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58DCA43F-452E-41CA-BDC7-EE0DB0E49D3E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{93745E4E-04A9-434F-98AB-2B1B4C6A22F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1162,36 +1162,12 @@
     <t>static/images/Puzzle_108.jpg</t>
   </si>
   <si>
-    <t>static/images/Puzzle_109.jpg</t>
-  </si>
-  <si>
     <t>static/images/Puzzle_110.jpg</t>
   </si>
   <si>
     <t>static/images/Puzzle_111.jpg</t>
   </si>
   <si>
-    <t>static/images/Puzzle_112.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_113.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_114.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_115.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_116.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_117.jpg</t>
-  </si>
-  <si>
-    <t>static/images/Puzzle_118.jpg</t>
-  </si>
-  <si>
     <t>static/images/Puzzle_119.jpg</t>
   </si>
   <si>
@@ -1222,9 +1198,6 @@
     <t>static/images/Puzzle_128.jpg</t>
   </si>
   <si>
-    <t>static/images/Puzzle_129.jpg</t>
-  </si>
-  <si>
     <t>static/images/Puzzle_130.jpg</t>
   </si>
   <si>
@@ -1276,9 +1249,6 @@
     <t>static/images/Puzzle_146.jpg</t>
   </si>
   <si>
-    <t>static/images/Puzzle_147.jpg</t>
-  </si>
-  <si>
     <t>static/images/Puzzle_148.jpg</t>
   </si>
   <si>
@@ -1367,6 +1337,36 @@
   </si>
   <si>
     <t>static/images/Puzzle_006.jpg</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_109.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_112.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_113.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_114.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_115.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_116.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_117.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_118.JPG</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_129.jpeg</t>
+  </si>
+  <si>
+    <t>static/images/Puzzle_147.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1732,9 +1732,9 @@
   <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,7 +1915,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2415,7 +2415,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C28">
         <v>500</v>
@@ -4412,11 +4412,11 @@
         <v>167</v>
       </c>
       <c r="F110" t="s">
-        <v>374</v>
+        <v>433</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "static/images/Puzzle_109.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "109","Title": "Dining Mickey &amp; Minnie","Pieces": "500","Company": "Ceaco","Size": "18 X 14","URL": "static/images/Puzzle_109.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -4436,7 +4436,7 @@
         <v>171</v>
       </c>
       <c r="F111" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
@@ -4460,7 +4460,7 @@
         <v>171</v>
       </c>
       <c r="F112" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
@@ -4484,11 +4484,11 @@
         <v>175</v>
       </c>
       <c r="F113" t="s">
-        <v>377</v>
+        <v>434</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "static/images/Puzzle_112.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "112","Title": "Grand Canyon National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "static/images/Puzzle_112.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
@@ -4508,11 +4508,11 @@
         <v>91</v>
       </c>
       <c r="F114" t="s">
-        <v>378</v>
+        <v>435</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_113.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "113","Title": "Bryce National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_113.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
@@ -4532,11 +4532,11 @@
         <v>178</v>
       </c>
       <c r="F115" t="s">
-        <v>379</v>
+        <v>436</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "static/images/Puzzle_114.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "114","Title": "Grand Teton National Park","Pieces": "1000","Company": "Professor Puzzle","Size": "29 X 19","URL": "static/images/Puzzle_114.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -4556,11 +4556,11 @@
         <v>91</v>
       </c>
       <c r="F116" t="s">
-        <v>380</v>
+        <v>437</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_115.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "115","Title": "Yosemite National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_115.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
@@ -4580,11 +4580,11 @@
         <v>91</v>
       </c>
       <c r="F117" t="s">
-        <v>381</v>
+        <v>438</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_116.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "116","Title": "Joshua Tree National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_116.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -4604,11 +4604,11 @@
         <v>175</v>
       </c>
       <c r="F118" t="s">
-        <v>382</v>
+        <v>439</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "static/images/Puzzle_117.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "117","Title": "Yellowstone National Park","Pieces": "750","Company": "Professor Puzzle","Size": "24 X 15","URL": "static/images/Puzzle_117.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
@@ -4628,11 +4628,11 @@
         <v>91</v>
       </c>
       <c r="F119" t="s">
-        <v>383</v>
+        <v>440</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_118.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "118","Title": "Glacier National Park","Pieces": "500","Company": "Professor Puzzle","Size": "19 X 14","URL": "static/images/Puzzle_118.JPG","Missing":""},</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
@@ -4649,7 +4649,7 @@
         <v>184</v>
       </c>
       <c r="F120" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
@@ -4673,7 +4673,7 @@
         <v>186</v>
       </c>
       <c r="F121" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
@@ -4697,7 +4697,7 @@
         <v>120</v>
       </c>
       <c r="F122" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
@@ -4721,7 +4721,7 @@
         <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
@@ -4745,7 +4745,7 @@
         <v>41</v>
       </c>
       <c r="F124" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
@@ -4769,7 +4769,7 @@
         <v>192</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" t="str">
@@ -4794,7 +4794,7 @@
         <v>192</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" t="str">
@@ -4819,7 +4819,7 @@
         <v>192</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="str">
@@ -4844,7 +4844,7 @@
         <v>34</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" t="str">
@@ -4869,7 +4869,7 @@
         <v>198</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" t="str">
@@ -4894,12 +4894,12 @@
         <v>78</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>394</v>
+        <v>441</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" t="str">
         <f t="shared" si="1"/>
-        <v>{"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "static/images/Puzzle_129.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "129","Title": "Disney 1951: Alice","Pieces": "1000","Company": "Ravensburger","Size": "27 X 20","URL": "static/images/Puzzle_129.jpeg","Missing":""},</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -4919,7 +4919,7 @@
         <v>7</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="G131" s="1"/>
       <c r="H131" t="str">
@@ -4944,7 +4944,7 @@
         <v>78</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" t="str">
@@ -4969,7 +4969,7 @@
         <v>131</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="G133" s="1"/>
       <c r="H133" t="str">
@@ -4994,7 +4994,7 @@
         <v>26</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" t="str">
@@ -5019,7 +5019,7 @@
         <v>26</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" t="str">
@@ -5044,7 +5044,7 @@
         <v>7</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" t="str">
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" t="str">
@@ -5094,7 +5094,7 @@
         <v>192</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" t="str">
@@ -5119,7 +5119,7 @@
         <v>78</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" t="str">
@@ -5144,7 +5144,7 @@
         <v>91</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="G140" s="1"/>
       <c r="H140" t="str">
@@ -5169,7 +5169,7 @@
         <v>91</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" t="str">
@@ -5191,7 +5191,7 @@
         <v>214</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="G142" s="1"/>
       <c r="H142" t="str">
@@ -5216,7 +5216,7 @@
         <v>216</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" t="str">
@@ -5241,7 +5241,7 @@
         <v>7</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" t="str">
@@ -5266,7 +5266,7 @@
         <v>78</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="G145" s="1"/>
       <c r="H145" t="str">
@@ -5291,7 +5291,7 @@
         <v>78</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="G146" s="1"/>
       <c r="H146" t="str">
@@ -5316,7 +5316,7 @@
         <v>91</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="G147" s="1"/>
       <c r="H147" t="str">
@@ -5341,12 +5341,12 @@
         <v>222</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>412</v>
+        <v>442</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
-        <v>{"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "static/images/Puzzle_147.jpg","Missing":""},</v>
+        <v>{"PuzzleNum": "147","Title": "Dr. Suess","Pieces": "1000","Company": "The OP Puzzles","Size": "19 X 27","URL": "static/images/Puzzle_147.jpeg","Missing":""},</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -5366,7 +5366,7 @@
         <v>7</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="G149" s="1"/>
       <c r="H149" t="str">
@@ -5391,7 +5391,7 @@
         <v>7</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" t="str">
@@ -5416,7 +5416,7 @@
         <v>7</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="G151" s="1"/>
       <c r="H151" t="str">
@@ -5441,7 +5441,7 @@
         <v>227</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="G152" s="1"/>
       <c r="H152" t="str">
@@ -5466,7 +5466,7 @@
         <v>34</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="G153" s="1"/>
       <c r="H153" t="str">
@@ -5491,7 +5491,7 @@
         <v>94</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="G154" s="1"/>
       <c r="H154" t="str">
@@ -5516,7 +5516,7 @@
         <v>78</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" t="str">
@@ -5541,7 +5541,7 @@
         <v>198</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="G156" s="1"/>
       <c r="H156" t="str">
@@ -5566,7 +5566,7 @@
         <v>233</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="G157" s="1"/>
       <c r="H157" t="str">
@@ -5591,7 +5591,7 @@
         <v>34</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="G158" s="1"/>
       <c r="H158" t="str">
@@ -5616,7 +5616,7 @@
         <v>7</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="G159" s="1"/>
       <c r="H159" t="str">
@@ -5641,7 +5641,7 @@
         <v>216</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G160" s="1"/>
       <c r="H160" t="str">
@@ -5666,7 +5666,7 @@
         <v>238</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="G161" s="1"/>
       <c r="H161" t="str">
@@ -5691,7 +5691,7 @@
         <v>216</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="G162" s="1"/>
       <c r="H162" t="str">
@@ -5716,7 +5716,7 @@
         <v>238</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G163" s="1"/>
       <c r="H163" t="str">
@@ -5741,7 +5741,7 @@
         <v>243</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="G164" s="1"/>
       <c r="H164" t="str">
@@ -5766,7 +5766,7 @@
         <v>245</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="G165" s="1"/>
       <c r="H165" t="str">
@@ -5791,7 +5791,7 @@
         <v>216</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="G166" s="1"/>
       <c r="H166" t="str">
@@ -5816,7 +5816,7 @@
         <v>26</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="G167" s="1"/>
       <c r="H167" t="str">
@@ -5841,7 +5841,7 @@
         <v>216</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="G168" s="1"/>
       <c r="H168" t="str">
@@ -5866,7 +5866,7 @@
         <v>259</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="G169" s="1"/>
       <c r="H169" t="str">
@@ -5891,7 +5891,7 @@
         <v>147</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="G170" s="1"/>
       <c r="H170" t="str">
@@ -5916,7 +5916,7 @@
         <v>261</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="G171" s="1"/>
       <c r="H171" t="str">
@@ -5941,7 +5941,7 @@
         <v>10</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G172" s="1"/>
       <c r="H172" t="str">
@@ -5966,7 +5966,7 @@
         <v>137</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="G173" s="1"/>
       <c r="H173" t="str">
@@ -5991,7 +5991,7 @@
         <v>263</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="G174" s="1"/>
       <c r="H174" t="str">
@@ -6016,7 +6016,7 @@
         <v>265</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="G175" s="1"/>
       <c r="H175" t="str">
@@ -6041,7 +6041,7 @@
         <v>78</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" t="str">

</xml_diff>